<commit_message>
Convert to static site
</commit_message>
<xml_diff>
--- a/static/data/confidence_indices.xlsx
+++ b/static/data/confidence_indices.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -452,7 +452,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I437"/>
+  <dimension ref="A1:I438"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11519,25 +11519,25 @@
         <v>83.33333333333334</v>
       </c>
       <c r="C434" t="n">
-        <v>50</v>
+        <v>54.16666666666666</v>
       </c>
       <c r="D434" t="n">
         <v>33.33333333333333</v>
       </c>
       <c r="E434" t="n">
-        <v>23.07692307692308</v>
+        <v>25</v>
       </c>
       <c r="F434" t="n">
         <v>77.77777777777779</v>
       </c>
       <c r="G434" t="n">
-        <v>19.04761904761905</v>
+        <v>26.08695652173913</v>
       </c>
       <c r="H434" t="n">
         <v>66.66666666666666</v>
       </c>
       <c r="I434" t="n">
-        <v>29.16666666666667</v>
+        <v>26.92307692307692</v>
       </c>
     </row>
     <row r="435">
@@ -11548,25 +11548,25 @@
         <v>63.63636363636363</v>
       </c>
       <c r="C435" t="n">
-        <v>82.60869565217391</v>
+        <v>79.16666666666666</v>
       </c>
       <c r="D435" t="n">
         <v>7.692307692307693</v>
       </c>
       <c r="E435" t="n">
-        <v>27.58620689655172</v>
+        <v>26.66666666666667</v>
       </c>
       <c r="F435" t="n">
         <v>54.54545454545454</v>
       </c>
       <c r="G435" t="n">
-        <v>69.23076923076923</v>
+        <v>70.37037037037037</v>
       </c>
       <c r="H435" t="n">
         <v>25</v>
       </c>
       <c r="I435" t="n">
-        <v>55.55555555555556</v>
+        <v>57.14285714285714</v>
       </c>
     </row>
     <row r="436">
@@ -11603,28 +11603,57 @@
         <v>45869</v>
       </c>
       <c r="B437" t="n">
-        <v>60</v>
+        <v>57.14285714285714</v>
       </c>
       <c r="C437" t="n">
-        <v>84</v>
+        <v>81.48148148148148</v>
       </c>
       <c r="D437" t="n">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="E437" t="n">
-        <v>44.44444444444444</v>
+        <v>42.85714285714285</v>
       </c>
       <c r="F437" t="n">
-        <v>42.85714285714285</v>
+        <v>50</v>
       </c>
       <c r="G437" t="n">
-        <v>60</v>
+        <v>61.90476190476191</v>
       </c>
       <c r="H437" t="n">
-        <v>55.55555555555556</v>
+        <v>54.54545454545454</v>
       </c>
       <c r="I437" t="n">
-        <v>36.36363636363637</v>
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" s="2" t="n">
+        <v>45900</v>
+      </c>
+      <c r="B438" t="n">
+        <v>50</v>
+      </c>
+      <c r="C438" t="n">
+        <v>76.19047619047619</v>
+      </c>
+      <c r="D438" t="n">
+        <v>26.66666666666667</v>
+      </c>
+      <c r="E438" t="n">
+        <v>52.17391304347826</v>
+      </c>
+      <c r="F438" t="n">
+        <v>76.92307692307693</v>
+      </c>
+      <c r="G438" t="n">
+        <v>70</v>
+      </c>
+      <c r="H438" t="n">
+        <v>20</v>
+      </c>
+      <c r="I438" t="n">
+        <v>45.45454545454545</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Convert to static site (Sep 2025)
</commit_message>
<xml_diff>
--- a/static/data/confidence_indices.xlsx
+++ b/static/data/confidence_indices.xlsx
@@ -20,16 +20,13 @@
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
     <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -40,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -48,45 +45,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -452,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I438"/>
+  <dimension ref="A1:I439"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,84 +426,80 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr"/>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr"/>
+      <c r="B1" t="inlineStr">
         <is>
           <t>1-Year Confidence</t>
         </is>
       </c>
-      <c r="C1" s="1" t="n"/>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>Crash Confidence</t>
         </is>
       </c>
-      <c r="E1" s="1" t="n"/>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>Buy-On-Dips Confidence</t>
         </is>
       </c>
-      <c r="G1" s="1" t="n"/>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>Valuation Confidence</t>
         </is>
       </c>
-      <c r="I1" s="1" t="n"/>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr"/>
-      <c r="B2" s="1" t="inlineStr">
+      <c r="A2" t="inlineStr"/>
+      <c r="B2" t="inlineStr">
         <is>
           <t>Corporate</t>
         </is>
       </c>
-      <c r="C2" s="1" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>Individual</t>
         </is>
       </c>
-      <c r="D2" s="1" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>Corporate</t>
         </is>
       </c>
-      <c r="E2" s="1" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>Individual</t>
         </is>
       </c>
-      <c r="F2" s="1" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>Corporate</t>
         </is>
       </c>
-      <c r="G2" s="1" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>Individual</t>
         </is>
       </c>
-      <c r="H2" s="1" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>Corporate</t>
         </is>
       </c>
-      <c r="I2" s="1" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>Individual</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
+      <c r="A3" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="n">
+      <c r="A4" s="1" t="n">
         <v>32689</v>
       </c>
       <c r="B4" t="n">
@@ -559,7 +520,7 @@
       <c r="I4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="n">
+      <c r="A5" s="1" t="n">
         <v>32720</v>
       </c>
       <c r="B5" t="n">
@@ -588,7 +549,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="n">
+      <c r="A6" s="1" t="n">
         <v>32751</v>
       </c>
       <c r="B6" t="n">
@@ -617,7 +578,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="n">
+      <c r="A7" s="1" t="n">
         <v>32781</v>
       </c>
       <c r="B7" t="inlineStr"/>
@@ -630,7 +591,7 @@
       <c r="I7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="n">
+      <c r="A8" s="1" t="n">
         <v>32812</v>
       </c>
       <c r="B8" t="inlineStr"/>
@@ -643,7 +604,7 @@
       <c r="I8" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="n">
+      <c r="A9" s="1" t="n">
         <v>32842</v>
       </c>
       <c r="B9" t="inlineStr"/>
@@ -656,7 +617,7 @@
       <c r="I9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="n">
+      <c r="A10" s="1" t="n">
         <v>32873</v>
       </c>
       <c r="B10" t="inlineStr"/>
@@ -669,7 +630,7 @@
       <c r="I10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" s="2" t="n">
+      <c r="A11" s="1" t="n">
         <v>32904</v>
       </c>
       <c r="B11" t="n">
@@ -690,7 +651,7 @@
       <c r="I11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" s="2" t="n">
+      <c r="A12" s="1" t="n">
         <v>32932</v>
       </c>
       <c r="B12" t="n">
@@ -711,7 +672,7 @@
       <c r="I12" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" s="2" t="n">
+      <c r="A13" s="1" t="n">
         <v>32963</v>
       </c>
       <c r="B13" t="n">
@@ -732,7 +693,7 @@
       <c r="I13" t="inlineStr"/>
     </row>
     <row r="14">
-      <c r="A14" s="2" t="n">
+      <c r="A14" s="1" t="n">
         <v>32993</v>
       </c>
       <c r="B14" t="inlineStr"/>
@@ -745,7 +706,7 @@
       <c r="I14" t="inlineStr"/>
     </row>
     <row r="15">
-      <c r="A15" s="2" t="n">
+      <c r="A15" s="1" t="n">
         <v>33024</v>
       </c>
       <c r="B15" t="inlineStr"/>
@@ -758,7 +719,7 @@
       <c r="I15" t="inlineStr"/>
     </row>
     <row r="16">
-      <c r="A16" s="2" t="n">
+      <c r="A16" s="1" t="n">
         <v>33054</v>
       </c>
       <c r="B16" t="inlineStr"/>
@@ -771,7 +732,7 @@
       <c r="I16" t="inlineStr"/>
     </row>
     <row r="17">
-      <c r="A17" s="2" t="n">
+      <c r="A17" s="1" t="n">
         <v>33085</v>
       </c>
       <c r="B17" t="n">
@@ -792,7 +753,7 @@
       <c r="I17" t="inlineStr"/>
     </row>
     <row r="18">
-      <c r="A18" s="2" t="n">
+      <c r="A18" s="1" t="n">
         <v>33116</v>
       </c>
       <c r="B18" t="n">
@@ -813,7 +774,7 @@
       <c r="I18" t="inlineStr"/>
     </row>
     <row r="19">
-      <c r="A19" s="2" t="n">
+      <c r="A19" s="1" t="n">
         <v>33146</v>
       </c>
       <c r="B19" t="n">
@@ -832,7 +793,7 @@
       <c r="I19" t="inlineStr"/>
     </row>
     <row r="20">
-      <c r="A20" s="2" t="n">
+      <c r="A20" s="1" t="n">
         <v>33177</v>
       </c>
       <c r="B20" t="inlineStr"/>
@@ -845,7 +806,7 @@
       <c r="I20" t="inlineStr"/>
     </row>
     <row r="21">
-      <c r="A21" s="2" t="n">
+      <c r="A21" s="1" t="n">
         <v>33207</v>
       </c>
       <c r="B21" t="inlineStr"/>
@@ -858,7 +819,7 @@
       <c r="I21" t="inlineStr"/>
     </row>
     <row r="22">
-      <c r="A22" s="2" t="n">
+      <c r="A22" s="1" t="n">
         <v>33238</v>
       </c>
       <c r="B22" t="inlineStr"/>
@@ -871,7 +832,7 @@
       <c r="I22" t="inlineStr"/>
     </row>
     <row r="23">
-      <c r="A23" s="2" t="n">
+      <c r="A23" s="1" t="n">
         <v>33269</v>
       </c>
       <c r="B23" t="n">
@@ -892,7 +853,7 @@
       <c r="I23" t="inlineStr"/>
     </row>
     <row r="24">
-      <c r="A24" s="2" t="n">
+      <c r="A24" s="1" t="n">
         <v>33297</v>
       </c>
       <c r="B24" t="n">
@@ -913,7 +874,7 @@
       <c r="I24" t="inlineStr"/>
     </row>
     <row r="25">
-      <c r="A25" s="2" t="n">
+      <c r="A25" s="1" t="n">
         <v>33328</v>
       </c>
       <c r="B25" t="n">
@@ -934,7 +895,7 @@
       <c r="I25" t="inlineStr"/>
     </row>
     <row r="26">
-      <c r="A26" s="2" t="n">
+      <c r="A26" s="1" t="n">
         <v>33358</v>
       </c>
       <c r="B26" t="n">
@@ -953,7 +914,7 @@
       <c r="I26" t="inlineStr"/>
     </row>
     <row r="27">
-      <c r="A27" s="2" t="n">
+      <c r="A27" s="1" t="n">
         <v>33389</v>
       </c>
       <c r="B27" t="inlineStr"/>
@@ -966,7 +927,7 @@
       <c r="I27" t="inlineStr"/>
     </row>
     <row r="28">
-      <c r="A28" s="2" t="n">
+      <c r="A28" s="1" t="n">
         <v>33419</v>
       </c>
       <c r="B28" t="inlineStr"/>
@@ -979,7 +940,7 @@
       <c r="I28" t="inlineStr"/>
     </row>
     <row r="29">
-      <c r="A29" s="2" t="n">
+      <c r="A29" s="1" t="n">
         <v>33450</v>
       </c>
       <c r="B29" t="inlineStr"/>
@@ -992,7 +953,7 @@
       <c r="I29" t="inlineStr"/>
     </row>
     <row r="30">
-      <c r="A30" s="2" t="n">
+      <c r="A30" s="1" t="n">
         <v>33481</v>
       </c>
       <c r="B30" t="n">
@@ -1013,7 +974,7 @@
       <c r="I30" t="inlineStr"/>
     </row>
     <row r="31">
-      <c r="A31" s="2" t="n">
+      <c r="A31" s="1" t="n">
         <v>33511</v>
       </c>
       <c r="B31" t="n">
@@ -1034,7 +995,7 @@
       <c r="I31" t="inlineStr"/>
     </row>
     <row r="32">
-      <c r="A32" s="2" t="n">
+      <c r="A32" s="1" t="n">
         <v>33542</v>
       </c>
       <c r="B32" t="n">
@@ -1055,7 +1016,7 @@
       <c r="I32" t="inlineStr"/>
     </row>
     <row r="33">
-      <c r="A33" s="2" t="n">
+      <c r="A33" s="1" t="n">
         <v>33572</v>
       </c>
       <c r="B33" t="inlineStr"/>
@@ -1068,7 +1029,7 @@
       <c r="I33" t="inlineStr"/>
     </row>
     <row r="34">
-      <c r="A34" s="2" t="n">
+      <c r="A34" s="1" t="n">
         <v>33603</v>
       </c>
       <c r="B34" t="inlineStr"/>
@@ -1081,7 +1042,7 @@
       <c r="I34" t="inlineStr"/>
     </row>
     <row r="35">
-      <c r="A35" s="2" t="n">
+      <c r="A35" s="1" t="n">
         <v>33634</v>
       </c>
       <c r="B35" t="n">
@@ -1098,7 +1059,7 @@
       <c r="I35" t="inlineStr"/>
     </row>
     <row r="36">
-      <c r="A36" s="2" t="n">
+      <c r="A36" s="1" t="n">
         <v>33663</v>
       </c>
       <c r="B36" t="n">
@@ -1119,7 +1080,7 @@
       <c r="I36" t="inlineStr"/>
     </row>
     <row r="37">
-      <c r="A37" s="2" t="n">
+      <c r="A37" s="1" t="n">
         <v>33694</v>
       </c>
       <c r="B37" t="n">
@@ -1140,7 +1101,7 @@
       <c r="I37" t="inlineStr"/>
     </row>
     <row r="38">
-      <c r="A38" s="2" t="n">
+      <c r="A38" s="1" t="n">
         <v>33724</v>
       </c>
       <c r="B38" t="n">
@@ -1159,7 +1120,7 @@
       <c r="I38" t="inlineStr"/>
     </row>
     <row r="39">
-      <c r="A39" s="2" t="n">
+      <c r="A39" s="1" t="n">
         <v>33755</v>
       </c>
       <c r="B39" t="inlineStr"/>
@@ -1172,7 +1133,7 @@
       <c r="I39" t="inlineStr"/>
     </row>
     <row r="40">
-      <c r="A40" s="2" t="n">
+      <c r="A40" s="1" t="n">
         <v>33785</v>
       </c>
       <c r="B40" t="inlineStr"/>
@@ -1185,7 +1146,7 @@
       <c r="I40" t="inlineStr"/>
     </row>
     <row r="41">
-      <c r="A41" s="2" t="n">
+      <c r="A41" s="1" t="n">
         <v>33816</v>
       </c>
       <c r="B41" t="inlineStr"/>
@@ -1198,7 +1159,7 @@
       <c r="I41" t="inlineStr"/>
     </row>
     <row r="42">
-      <c r="A42" s="2" t="n">
+      <c r="A42" s="1" t="n">
         <v>33847</v>
       </c>
       <c r="B42" t="n">
@@ -1219,7 +1180,7 @@
       <c r="I42" t="inlineStr"/>
     </row>
     <row r="43">
-      <c r="A43" s="2" t="n">
+      <c r="A43" s="1" t="n">
         <v>33877</v>
       </c>
       <c r="B43" t="n">
@@ -1240,7 +1201,7 @@
       <c r="I43" t="inlineStr"/>
     </row>
     <row r="44">
-      <c r="A44" s="2" t="n">
+      <c r="A44" s="1" t="n">
         <v>33908</v>
       </c>
       <c r="B44" t="n">
@@ -1259,7 +1220,7 @@
       <c r="I44" t="inlineStr"/>
     </row>
     <row r="45">
-      <c r="A45" s="2" t="n">
+      <c r="A45" s="1" t="n">
         <v>33938</v>
       </c>
       <c r="B45" t="inlineStr"/>
@@ -1272,7 +1233,7 @@
       <c r="I45" t="inlineStr"/>
     </row>
     <row r="46">
-      <c r="A46" s="2" t="n">
+      <c r="A46" s="1" t="n">
         <v>33969</v>
       </c>
       <c r="B46" t="inlineStr"/>
@@ -1285,7 +1246,7 @@
       <c r="I46" t="inlineStr"/>
     </row>
     <row r="47">
-      <c r="A47" s="2" t="n">
+      <c r="A47" s="1" t="n">
         <v>34000</v>
       </c>
       <c r="B47" t="inlineStr"/>
@@ -1298,7 +1259,7 @@
       <c r="I47" t="inlineStr"/>
     </row>
     <row r="48">
-      <c r="A48" s="2" t="n">
+      <c r="A48" s="1" t="n">
         <v>34028</v>
       </c>
       <c r="B48" t="n">
@@ -1319,7 +1280,7 @@
       <c r="I48" t="inlineStr"/>
     </row>
     <row r="49">
-      <c r="A49" s="2" t="n">
+      <c r="A49" s="1" t="n">
         <v>34059</v>
       </c>
       <c r="B49" t="n">
@@ -1340,7 +1301,7 @@
       <c r="I49" t="inlineStr"/>
     </row>
     <row r="50">
-      <c r="A50" s="2" t="n">
+      <c r="A50" s="1" t="n">
         <v>34089</v>
       </c>
       <c r="B50" t="n">
@@ -1361,7 +1322,7 @@
       <c r="I50" t="inlineStr"/>
     </row>
     <row r="51">
-      <c r="A51" s="2" t="n">
+      <c r="A51" s="1" t="n">
         <v>34120</v>
       </c>
       <c r="B51" t="inlineStr"/>
@@ -1374,7 +1335,7 @@
       <c r="I51" t="inlineStr"/>
     </row>
     <row r="52">
-      <c r="A52" s="2" t="n">
+      <c r="A52" s="1" t="n">
         <v>34150</v>
       </c>
       <c r="B52" t="inlineStr"/>
@@ -1387,7 +1348,7 @@
       <c r="I52" t="inlineStr"/>
     </row>
     <row r="53">
-      <c r="A53" s="2" t="n">
+      <c r="A53" s="1" t="n">
         <v>34181</v>
       </c>
       <c r="B53" t="inlineStr"/>
@@ -1400,7 +1361,7 @@
       <c r="I53" t="inlineStr"/>
     </row>
     <row r="54">
-      <c r="A54" s="2" t="n">
+      <c r="A54" s="1" t="n">
         <v>34212</v>
       </c>
       <c r="B54" t="n">
@@ -1421,7 +1382,7 @@
       <c r="I54" t="inlineStr"/>
     </row>
     <row r="55">
-      <c r="A55" s="2" t="n">
+      <c r="A55" s="1" t="n">
         <v>34242</v>
       </c>
       <c r="B55" t="n">
@@ -1442,7 +1403,7 @@
       <c r="I55" t="inlineStr"/>
     </row>
     <row r="56">
-      <c r="A56" s="2" t="n">
+      <c r="A56" s="1" t="n">
         <v>34273</v>
       </c>
       <c r="B56" t="n">
@@ -1463,7 +1424,7 @@
       <c r="I56" t="inlineStr"/>
     </row>
     <row r="57">
-      <c r="A57" s="2" t="n">
+      <c r="A57" s="1" t="n">
         <v>34303</v>
       </c>
       <c r="B57" t="inlineStr"/>
@@ -1476,7 +1437,7 @@
       <c r="I57" t="inlineStr"/>
     </row>
     <row r="58">
-      <c r="A58" s="2" t="n">
+      <c r="A58" s="1" t="n">
         <v>34334</v>
       </c>
       <c r="B58" t="inlineStr"/>
@@ -1489,7 +1450,7 @@
       <c r="I58" t="inlineStr"/>
     </row>
     <row r="59">
-      <c r="A59" s="2" t="n">
+      <c r="A59" s="1" t="n">
         <v>34365</v>
       </c>
       <c r="B59" t="inlineStr"/>
@@ -1502,7 +1463,7 @@
       <c r="I59" t="inlineStr"/>
     </row>
     <row r="60">
-      <c r="A60" s="2" t="n">
+      <c r="A60" s="1" t="n">
         <v>34393</v>
       </c>
       <c r="B60" t="n">
@@ -1523,7 +1484,7 @@
       <c r="I60" t="inlineStr"/>
     </row>
     <row r="61">
-      <c r="A61" s="2" t="n">
+      <c r="A61" s="1" t="n">
         <v>34424</v>
       </c>
       <c r="B61" t="n">
@@ -1544,7 +1505,7 @@
       <c r="I61" t="inlineStr"/>
     </row>
     <row r="62">
-      <c r="A62" s="2" t="n">
+      <c r="A62" s="1" t="n">
         <v>34454</v>
       </c>
       <c r="B62" t="n">
@@ -1565,7 +1526,7 @@
       <c r="I62" t="inlineStr"/>
     </row>
     <row r="63">
-      <c r="A63" s="2" t="n">
+      <c r="A63" s="1" t="n">
         <v>34485</v>
       </c>
       <c r="B63" t="inlineStr"/>
@@ -1578,7 +1539,7 @@
       <c r="I63" t="inlineStr"/>
     </row>
     <row r="64">
-      <c r="A64" s="2" t="n">
+      <c r="A64" s="1" t="n">
         <v>34515</v>
       </c>
       <c r="B64" t="inlineStr"/>
@@ -1591,7 +1552,7 @@
       <c r="I64" t="inlineStr"/>
     </row>
     <row r="65">
-      <c r="A65" s="2" t="n">
+      <c r="A65" s="1" t="n">
         <v>34546</v>
       </c>
       <c r="B65" t="inlineStr"/>
@@ -1604,7 +1565,7 @@
       <c r="I65" t="inlineStr"/>
     </row>
     <row r="66">
-      <c r="A66" s="2" t="n">
+      <c r="A66" s="1" t="n">
         <v>34577</v>
       </c>
       <c r="B66" t="inlineStr"/>
@@ -1617,7 +1578,7 @@
       <c r="I66" t="inlineStr"/>
     </row>
     <row r="67">
-      <c r="A67" s="2" t="n">
+      <c r="A67" s="1" t="n">
         <v>34607</v>
       </c>
       <c r="B67" t="n">
@@ -1638,7 +1599,7 @@
       <c r="I67" t="inlineStr"/>
     </row>
     <row r="68">
-      <c r="A68" s="2" t="n">
+      <c r="A68" s="1" t="n">
         <v>34638</v>
       </c>
       <c r="B68" t="n">
@@ -1659,7 +1620,7 @@
       <c r="I68" t="inlineStr"/>
     </row>
     <row r="69">
-      <c r="A69" s="2" t="n">
+      <c r="A69" s="1" t="n">
         <v>34668</v>
       </c>
       <c r="B69" t="n">
@@ -1680,7 +1641,7 @@
       <c r="I69" t="inlineStr"/>
     </row>
     <row r="70">
-      <c r="A70" s="2" t="n">
+      <c r="A70" s="1" t="n">
         <v>34699</v>
       </c>
       <c r="B70" t="inlineStr"/>
@@ -1693,7 +1654,7 @@
       <c r="I70" t="inlineStr"/>
     </row>
     <row r="71">
-      <c r="A71" s="2" t="n">
+      <c r="A71" s="1" t="n">
         <v>34730</v>
       </c>
       <c r="B71" t="inlineStr"/>
@@ -1706,7 +1667,7 @@
       <c r="I71" t="inlineStr"/>
     </row>
     <row r="72">
-      <c r="A72" s="2" t="n">
+      <c r="A72" s="1" t="n">
         <v>34758</v>
       </c>
       <c r="B72" t="inlineStr"/>
@@ -1719,7 +1680,7 @@
       <c r="I72" t="inlineStr"/>
     </row>
     <row r="73">
-      <c r="A73" s="2" t="n">
+      <c r="A73" s="1" t="n">
         <v>34789</v>
       </c>
       <c r="B73" t="n">
@@ -1740,7 +1701,7 @@
       <c r="I73" t="inlineStr"/>
     </row>
     <row r="74">
-      <c r="A74" s="2" t="n">
+      <c r="A74" s="1" t="n">
         <v>34819</v>
       </c>
       <c r="B74" t="n">
@@ -1761,7 +1722,7 @@
       <c r="I74" t="inlineStr"/>
     </row>
     <row r="75">
-      <c r="A75" s="2" t="n">
+      <c r="A75" s="1" t="n">
         <v>34850</v>
       </c>
       <c r="B75" t="inlineStr"/>
@@ -1774,7 +1735,7 @@
       <c r="I75" t="inlineStr"/>
     </row>
     <row r="76">
-      <c r="A76" s="2" t="n">
+      <c r="A76" s="1" t="n">
         <v>34880</v>
       </c>
       <c r="B76" t="inlineStr"/>
@@ -1787,7 +1748,7 @@
       <c r="I76" t="inlineStr"/>
     </row>
     <row r="77">
-      <c r="A77" s="2" t="n">
+      <c r="A77" s="1" t="n">
         <v>34911</v>
       </c>
       <c r="B77" t="inlineStr"/>
@@ -1800,7 +1761,7 @@
       <c r="I77" t="inlineStr"/>
     </row>
     <row r="78">
-      <c r="A78" s="2" t="n">
+      <c r="A78" s="1" t="n">
         <v>34942</v>
       </c>
       <c r="B78" t="n">
@@ -1819,7 +1780,7 @@
       <c r="I78" t="inlineStr"/>
     </row>
     <row r="79">
-      <c r="A79" s="2" t="n">
+      <c r="A79" s="1" t="n">
         <v>34972</v>
       </c>
       <c r="B79" t="n">
@@ -1840,7 +1801,7 @@
       <c r="I79" t="inlineStr"/>
     </row>
     <row r="80">
-      <c r="A80" s="2" t="n">
+      <c r="A80" s="1" t="n">
         <v>35003</v>
       </c>
       <c r="B80" t="n">
@@ -1861,7 +1822,7 @@
       <c r="I80" t="inlineStr"/>
     </row>
     <row r="81">
-      <c r="A81" s="2" t="n">
+      <c r="A81" s="1" t="n">
         <v>35033</v>
       </c>
       <c r="B81" t="n">
@@ -1882,7 +1843,7 @@
       <c r="I81" t="inlineStr"/>
     </row>
     <row r="82">
-      <c r="A82" s="2" t="n">
+      <c r="A82" s="1" t="n">
         <v>35064</v>
       </c>
       <c r="B82" t="inlineStr"/>
@@ -1895,7 +1856,7 @@
       <c r="I82" t="inlineStr"/>
     </row>
     <row r="83">
-      <c r="A83" s="2" t="n">
+      <c r="A83" s="1" t="n">
         <v>35095</v>
       </c>
       <c r="B83" t="inlineStr"/>
@@ -1908,7 +1869,7 @@
       <c r="I83" t="inlineStr"/>
     </row>
     <row r="84">
-      <c r="A84" s="2" t="n">
+      <c r="A84" s="1" t="n">
         <v>35124</v>
       </c>
       <c r="B84" t="inlineStr"/>
@@ -1921,7 +1882,7 @@
       <c r="I84" t="inlineStr"/>
     </row>
     <row r="85">
-      <c r="A85" s="2" t="n">
+      <c r="A85" s="1" t="n">
         <v>35155</v>
       </c>
       <c r="B85" t="n">
@@ -1942,7 +1903,7 @@
       <c r="I85" t="inlineStr"/>
     </row>
     <row r="86">
-      <c r="A86" s="2" t="n">
+      <c r="A86" s="1" t="n">
         <v>35185</v>
       </c>
       <c r="B86" t="n">
@@ -1963,7 +1924,7 @@
       <c r="I86" t="inlineStr"/>
     </row>
     <row r="87">
-      <c r="A87" s="2" t="n">
+      <c r="A87" s="1" t="n">
         <v>35216</v>
       </c>
       <c r="B87" t="inlineStr"/>
@@ -1976,7 +1937,7 @@
       <c r="I87" t="inlineStr"/>
     </row>
     <row r="88">
-      <c r="A88" s="2" t="n">
+      <c r="A88" s="1" t="n">
         <v>35246</v>
       </c>
       <c r="B88" t="inlineStr"/>
@@ -1989,7 +1950,7 @@
       <c r="I88" t="inlineStr"/>
     </row>
     <row r="89">
-      <c r="A89" s="2" t="n">
+      <c r="A89" s="1" t="n">
         <v>35277</v>
       </c>
       <c r="B89" t="inlineStr"/>
@@ -2002,7 +1963,7 @@
       <c r="I89" t="inlineStr"/>
     </row>
     <row r="90">
-      <c r="A90" s="2" t="n">
+      <c r="A90" s="1" t="n">
         <v>35308</v>
       </c>
       <c r="B90" t="n">
@@ -2023,7 +1984,7 @@
       <c r="I90" t="inlineStr"/>
     </row>
     <row r="91">
-      <c r="A91" s="2" t="n">
+      <c r="A91" s="1" t="n">
         <v>35338</v>
       </c>
       <c r="B91" t="n">
@@ -2052,7 +2013,7 @@
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="2" t="n">
+      <c r="A92" s="1" t="n">
         <v>35369</v>
       </c>
       <c r="B92" t="n">
@@ -2081,7 +2042,7 @@
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="2" t="n">
+      <c r="A93" s="1" t="n">
         <v>35399</v>
       </c>
       <c r="B93" t="inlineStr"/>
@@ -2102,7 +2063,7 @@
       </c>
     </row>
     <row r="94">
-      <c r="A94" s="2" t="n">
+      <c r="A94" s="1" t="n">
         <v>35430</v>
       </c>
       <c r="B94" t="inlineStr"/>
@@ -2115,7 +2076,7 @@
       <c r="I94" t="inlineStr"/>
     </row>
     <row r="95">
-      <c r="A95" s="2" t="n">
+      <c r="A95" s="1" t="n">
         <v>35461</v>
       </c>
       <c r="B95" t="inlineStr"/>
@@ -2128,7 +2089,7 @@
       <c r="I95" t="inlineStr"/>
     </row>
     <row r="96">
-      <c r="A96" s="2" t="n">
+      <c r="A96" s="1" t="n">
         <v>35489</v>
       </c>
       <c r="B96" t="inlineStr"/>
@@ -2141,7 +2102,7 @@
       <c r="I96" t="inlineStr"/>
     </row>
     <row r="97">
-      <c r="A97" s="2" t="n">
+      <c r="A97" s="1" t="n">
         <v>35520</v>
       </c>
       <c r="B97" t="n">
@@ -2162,7 +2123,7 @@
       <c r="I97" t="inlineStr"/>
     </row>
     <row r="98">
-      <c r="A98" s="2" t="n">
+      <c r="A98" s="1" t="n">
         <v>35550</v>
       </c>
       <c r="B98" t="n">
@@ -2183,7 +2144,7 @@
       <c r="I98" t="inlineStr"/>
     </row>
     <row r="99">
-      <c r="A99" s="2" t="n">
+      <c r="A99" s="1" t="n">
         <v>35581</v>
       </c>
       <c r="B99" t="inlineStr"/>
@@ -2196,7 +2157,7 @@
       <c r="I99" t="inlineStr"/>
     </row>
     <row r="100">
-      <c r="A100" s="2" t="n">
+      <c r="A100" s="1" t="n">
         <v>35611</v>
       </c>
       <c r="B100" t="n">
@@ -2217,7 +2178,7 @@
       <c r="I100" t="inlineStr"/>
     </row>
     <row r="101">
-      <c r="A101" s="2" t="n">
+      <c r="A101" s="1" t="n">
         <v>35642</v>
       </c>
       <c r="B101" t="inlineStr"/>
@@ -2230,7 +2191,7 @@
       <c r="I101" t="inlineStr"/>
     </row>
     <row r="102">
-      <c r="A102" s="2" t="n">
+      <c r="A102" s="1" t="n">
         <v>35673</v>
       </c>
       <c r="B102" t="inlineStr"/>
@@ -2243,7 +2204,7 @@
       <c r="I102" t="inlineStr"/>
     </row>
     <row r="103">
-      <c r="A103" s="2" t="n">
+      <c r="A103" s="1" t="n">
         <v>35703</v>
       </c>
       <c r="B103" t="n">
@@ -2264,7 +2225,7 @@
       <c r="I103" t="inlineStr"/>
     </row>
     <row r="104">
-      <c r="A104" s="2" t="n">
+      <c r="A104" s="1" t="n">
         <v>35734</v>
       </c>
       <c r="B104" t="n">
@@ -2285,7 +2246,7 @@
       <c r="I104" t="inlineStr"/>
     </row>
     <row r="105">
-      <c r="A105" s="2" t="n">
+      <c r="A105" s="1" t="n">
         <v>35764</v>
       </c>
       <c r="B105" t="inlineStr"/>
@@ -2298,7 +2259,7 @@
       <c r="I105" t="inlineStr"/>
     </row>
     <row r="106">
-      <c r="A106" s="2" t="n">
+      <c r="A106" s="1" t="n">
         <v>35795</v>
       </c>
       <c r="B106" t="inlineStr"/>
@@ -2311,7 +2272,7 @@
       <c r="I106" t="inlineStr"/>
     </row>
     <row r="107">
-      <c r="A107" s="2" t="n">
+      <c r="A107" s="1" t="n">
         <v>35826</v>
       </c>
       <c r="B107" t="inlineStr"/>
@@ -2324,7 +2285,7 @@
       <c r="I107" t="inlineStr"/>
     </row>
     <row r="108">
-      <c r="A108" s="2" t="n">
+      <c r="A108" s="1" t="n">
         <v>35854</v>
       </c>
       <c r="B108" t="inlineStr"/>
@@ -2337,7 +2298,7 @@
       <c r="I108" t="inlineStr"/>
     </row>
     <row r="109">
-      <c r="A109" s="2" t="n">
+      <c r="A109" s="1" t="n">
         <v>35885</v>
       </c>
       <c r="B109" t="n">
@@ -2358,7 +2319,7 @@
       <c r="I109" t="inlineStr"/>
     </row>
     <row r="110">
-      <c r="A110" s="2" t="n">
+      <c r="A110" s="1" t="n">
         <v>35915</v>
       </c>
       <c r="B110" t="n">
@@ -2379,7 +2340,7 @@
       <c r="I110" t="inlineStr"/>
     </row>
     <row r="111">
-      <c r="A111" s="2" t="n">
+      <c r="A111" s="1" t="n">
         <v>35946</v>
       </c>
       <c r="B111" t="n">
@@ -2400,7 +2361,7 @@
       <c r="I111" t="inlineStr"/>
     </row>
     <row r="112">
-      <c r="A112" s="2" t="n">
+      <c r="A112" s="1" t="n">
         <v>35976</v>
       </c>
       <c r="B112" t="inlineStr"/>
@@ -2413,7 +2374,7 @@
       <c r="I112" t="inlineStr"/>
     </row>
     <row r="113">
-      <c r="A113" s="2" t="n">
+      <c r="A113" s="1" t="n">
         <v>36007</v>
       </c>
       <c r="B113" t="inlineStr"/>
@@ -2426,7 +2387,7 @@
       <c r="I113" t="inlineStr"/>
     </row>
     <row r="114">
-      <c r="A114" s="2" t="n">
+      <c r="A114" s="1" t="n">
         <v>36038</v>
       </c>
       <c r="B114" t="inlineStr"/>
@@ -2439,7 +2400,7 @@
       <c r="I114" t="inlineStr"/>
     </row>
     <row r="115">
-      <c r="A115" s="2" t="n">
+      <c r="A115" s="1" t="n">
         <v>36068</v>
       </c>
       <c r="B115" t="n">
@@ -2460,7 +2421,7 @@
       <c r="I115" t="inlineStr"/>
     </row>
     <row r="116">
-      <c r="A116" s="2" t="n">
+      <c r="A116" s="1" t="n">
         <v>36099</v>
       </c>
       <c r="B116" t="n">
@@ -2481,7 +2442,7 @@
       <c r="I116" t="inlineStr"/>
     </row>
     <row r="117">
-      <c r="A117" s="2" t="n">
+      <c r="A117" s="1" t="n">
         <v>36129</v>
       </c>
       <c r="B117" t="n">
@@ -2502,7 +2463,7 @@
       <c r="I117" t="inlineStr"/>
     </row>
     <row r="118">
-      <c r="A118" s="2" t="n">
+      <c r="A118" s="1" t="n">
         <v>36160</v>
       </c>
       <c r="B118" t="n">
@@ -2521,7 +2482,7 @@
       <c r="I118" t="inlineStr"/>
     </row>
     <row r="119">
-      <c r="A119" s="2" t="n">
+      <c r="A119" s="1" t="n">
         <v>36191</v>
       </c>
       <c r="B119" t="n">
@@ -2550,7 +2511,7 @@
       </c>
     </row>
     <row r="120">
-      <c r="A120" s="2" t="n">
+      <c r="A120" s="1" t="n">
         <v>36219</v>
       </c>
       <c r="B120" t="n">
@@ -2579,7 +2540,7 @@
       </c>
     </row>
     <row r="121">
-      <c r="A121" s="2" t="n">
+      <c r="A121" s="1" t="n">
         <v>36250</v>
       </c>
       <c r="B121" t="n">
@@ -2608,7 +2569,7 @@
       </c>
     </row>
     <row r="122">
-      <c r="A122" s="2" t="n">
+      <c r="A122" s="1" t="n">
         <v>36280</v>
       </c>
       <c r="B122" t="n">
@@ -2637,7 +2598,7 @@
       </c>
     </row>
     <row r="123">
-      <c r="A123" s="2" t="n">
+      <c r="A123" s="1" t="n">
         <v>36311</v>
       </c>
       <c r="B123" t="n">
@@ -2666,7 +2627,7 @@
       </c>
     </row>
     <row r="124">
-      <c r="A124" s="2" t="n">
+      <c r="A124" s="1" t="n">
         <v>36341</v>
       </c>
       <c r="B124" t="n">
@@ -2695,7 +2656,7 @@
       </c>
     </row>
     <row r="125">
-      <c r="A125" s="2" t="n">
+      <c r="A125" s="1" t="n">
         <v>36372</v>
       </c>
       <c r="B125" t="n">
@@ -2724,7 +2685,7 @@
       </c>
     </row>
     <row r="126">
-      <c r="A126" s="2" t="n">
+      <c r="A126" s="1" t="n">
         <v>36403</v>
       </c>
       <c r="B126" t="n">
@@ -2753,7 +2714,7 @@
       </c>
     </row>
     <row r="127">
-      <c r="A127" s="2" t="n">
+      <c r="A127" s="1" t="n">
         <v>36433</v>
       </c>
       <c r="B127" t="n">
@@ -2782,7 +2743,7 @@
       </c>
     </row>
     <row r="128">
-      <c r="A128" s="2" t="n">
+      <c r="A128" s="1" t="n">
         <v>36464</v>
       </c>
       <c r="B128" t="n">
@@ -2811,7 +2772,7 @@
       </c>
     </row>
     <row r="129">
-      <c r="A129" s="2" t="n">
+      <c r="A129" s="1" t="n">
         <v>36494</v>
       </c>
       <c r="B129" t="n">
@@ -2840,7 +2801,7 @@
       </c>
     </row>
     <row r="130">
-      <c r="A130" s="2" t="n">
+      <c r="A130" s="1" t="n">
         <v>36525</v>
       </c>
       <c r="B130" t="n">
@@ -2869,7 +2830,7 @@
       </c>
     </row>
     <row r="131">
-      <c r="A131" s="2" t="n">
+      <c r="A131" s="1" t="n">
         <v>36556</v>
       </c>
       <c r="B131" t="n">
@@ -2898,7 +2859,7 @@
       </c>
     </row>
     <row r="132">
-      <c r="A132" s="2" t="n">
+      <c r="A132" s="1" t="n">
         <v>36585</v>
       </c>
       <c r="B132" t="n">
@@ -2927,7 +2888,7 @@
       </c>
     </row>
     <row r="133">
-      <c r="A133" s="2" t="n">
+      <c r="A133" s="1" t="n">
         <v>36616</v>
       </c>
       <c r="B133" t="n">
@@ -2956,7 +2917,7 @@
       </c>
     </row>
     <row r="134">
-      <c r="A134" s="2" t="n">
+      <c r="A134" s="1" t="n">
         <v>36646</v>
       </c>
       <c r="B134" t="inlineStr"/>
@@ -2981,7 +2942,7 @@
       </c>
     </row>
     <row r="135">
-      <c r="A135" s="2" t="n">
+      <c r="A135" s="1" t="n">
         <v>36677</v>
       </c>
       <c r="B135" t="n">
@@ -3010,7 +2971,7 @@
       </c>
     </row>
     <row r="136">
-      <c r="A136" s="2" t="n">
+      <c r="A136" s="1" t="n">
         <v>36707</v>
       </c>
       <c r="B136" t="n">
@@ -3039,7 +3000,7 @@
       </c>
     </row>
     <row r="137">
-      <c r="A137" s="2" t="n">
+      <c r="A137" s="1" t="n">
         <v>36738</v>
       </c>
       <c r="B137" t="n">
@@ -3068,7 +3029,7 @@
       </c>
     </row>
     <row r="138">
-      <c r="A138" s="2" t="n">
+      <c r="A138" s="1" t="n">
         <v>36769</v>
       </c>
       <c r="B138" t="n">
@@ -3097,7 +3058,7 @@
       </c>
     </row>
     <row r="139">
-      <c r="A139" s="2" t="n">
+      <c r="A139" s="1" t="n">
         <v>36799</v>
       </c>
       <c r="B139" t="inlineStr"/>
@@ -3110,7 +3071,7 @@
       <c r="I139" t="inlineStr"/>
     </row>
     <row r="140">
-      <c r="A140" s="2" t="n">
+      <c r="A140" s="1" t="n">
         <v>36830</v>
       </c>
       <c r="B140" t="inlineStr"/>
@@ -3123,7 +3084,7 @@
       <c r="I140" t="inlineStr"/>
     </row>
     <row r="141">
-      <c r="A141" s="2" t="n">
+      <c r="A141" s="1" t="n">
         <v>36860</v>
       </c>
       <c r="B141" t="inlineStr"/>
@@ -3136,7 +3097,7 @@
       <c r="I141" t="inlineStr"/>
     </row>
     <row r="142">
-      <c r="A142" s="2" t="n">
+      <c r="A142" s="1" t="n">
         <v>36891</v>
       </c>
       <c r="B142" t="inlineStr"/>
@@ -3149,7 +3110,7 @@
       <c r="I142" t="inlineStr"/>
     </row>
     <row r="143">
-      <c r="A143" s="2" t="n">
+      <c r="A143" s="1" t="n">
         <v>36922</v>
       </c>
       <c r="B143" t="n">
@@ -3168,7 +3129,7 @@
       <c r="I143" t="inlineStr"/>
     </row>
     <row r="144">
-      <c r="A144" s="2" t="n">
+      <c r="A144" s="1" t="n">
         <v>36950</v>
       </c>
       <c r="B144" t="inlineStr"/>
@@ -3181,7 +3142,7 @@
       <c r="I144" t="inlineStr"/>
     </row>
     <row r="145">
-      <c r="A145" s="2" t="n">
+      <c r="A145" s="1" t="n">
         <v>36981</v>
       </c>
       <c r="B145" t="inlineStr"/>
@@ -3194,7 +3155,7 @@
       <c r="I145" t="inlineStr"/>
     </row>
     <row r="146">
-      <c r="A146" s="2" t="n">
+      <c r="A146" s="1" t="n">
         <v>37011</v>
       </c>
       <c r="B146" t="n">
@@ -3223,7 +3184,7 @@
       </c>
     </row>
     <row r="147">
-      <c r="A147" s="2" t="n">
+      <c r="A147" s="1" t="n">
         <v>37042</v>
       </c>
       <c r="B147" t="n">
@@ -3252,7 +3213,7 @@
       </c>
     </row>
     <row r="148">
-      <c r="A148" s="2" t="n">
+      <c r="A148" s="1" t="n">
         <v>37072</v>
       </c>
       <c r="B148" t="n">
@@ -3281,7 +3242,7 @@
       </c>
     </row>
     <row r="149">
-      <c r="A149" s="2" t="n">
+      <c r="A149" s="1" t="n">
         <v>37103</v>
       </c>
       <c r="B149" t="n">
@@ -3310,7 +3271,7 @@
       </c>
     </row>
     <row r="150">
-      <c r="A150" s="2" t="n">
+      <c r="A150" s="1" t="n">
         <v>37134</v>
       </c>
       <c r="B150" t="n">
@@ -3339,7 +3300,7 @@
       </c>
     </row>
     <row r="151">
-      <c r="A151" s="2" t="n">
+      <c r="A151" s="1" t="n">
         <v>37164</v>
       </c>
       <c r="B151" t="n">
@@ -3368,7 +3329,7 @@
       </c>
     </row>
     <row r="152">
-      <c r="A152" s="2" t="n">
+      <c r="A152" s="1" t="n">
         <v>37195</v>
       </c>
       <c r="B152" t="n">
@@ -3397,7 +3358,7 @@
       </c>
     </row>
     <row r="153">
-      <c r="A153" s="2" t="n">
+      <c r="A153" s="1" t="n">
         <v>37225</v>
       </c>
       <c r="B153" t="n">
@@ -3426,7 +3387,7 @@
       </c>
     </row>
     <row r="154">
-      <c r="A154" s="2" t="n">
+      <c r="A154" s="1" t="n">
         <v>37256</v>
       </c>
       <c r="B154" t="n">
@@ -3455,7 +3416,7 @@
       </c>
     </row>
     <row r="155">
-      <c r="A155" s="2" t="n">
+      <c r="A155" s="1" t="n">
         <v>37287</v>
       </c>
       <c r="B155" t="n">
@@ -3484,7 +3445,7 @@
       </c>
     </row>
     <row r="156">
-      <c r="A156" s="2" t="n">
+      <c r="A156" s="1" t="n">
         <v>37315</v>
       </c>
       <c r="B156" t="n">
@@ -3513,7 +3474,7 @@
       </c>
     </row>
     <row r="157">
-      <c r="A157" s="2" t="n">
+      <c r="A157" s="1" t="n">
         <v>37346</v>
       </c>
       <c r="B157" t="n">
@@ -3542,7 +3503,7 @@
       </c>
     </row>
     <row r="158">
-      <c r="A158" s="2" t="n">
+      <c r="A158" s="1" t="n">
         <v>37376</v>
       </c>
       <c r="B158" t="n">
@@ -3571,7 +3532,7 @@
       </c>
     </row>
     <row r="159">
-      <c r="A159" s="2" t="n">
+      <c r="A159" s="1" t="n">
         <v>37407</v>
       </c>
       <c r="B159" t="n">
@@ -3600,7 +3561,7 @@
       </c>
     </row>
     <row r="160">
-      <c r="A160" s="2" t="n">
+      <c r="A160" s="1" t="n">
         <v>37437</v>
       </c>
       <c r="B160" t="n">
@@ -3629,7 +3590,7 @@
       </c>
     </row>
     <row r="161">
-      <c r="A161" s="2" t="n">
+      <c r="A161" s="1" t="n">
         <v>37468</v>
       </c>
       <c r="B161" t="n">
@@ -3658,7 +3619,7 @@
       </c>
     </row>
     <row r="162">
-      <c r="A162" s="2" t="n">
+      <c r="A162" s="1" t="n">
         <v>37499</v>
       </c>
       <c r="B162" t="n">
@@ -3687,7 +3648,7 @@
       </c>
     </row>
     <row r="163">
-      <c r="A163" s="2" t="n">
+      <c r="A163" s="1" t="n">
         <v>37529</v>
       </c>
       <c r="B163" t="n">
@@ -3716,7 +3677,7 @@
       </c>
     </row>
     <row r="164">
-      <c r="A164" s="2" t="n">
+      <c r="A164" s="1" t="n">
         <v>37560</v>
       </c>
       <c r="B164" t="n">
@@ -3745,7 +3706,7 @@
       </c>
     </row>
     <row r="165">
-      <c r="A165" s="2" t="n">
+      <c r="A165" s="1" t="n">
         <v>37590</v>
       </c>
       <c r="B165" t="n">
@@ -3774,7 +3735,7 @@
       </c>
     </row>
     <row r="166">
-      <c r="A166" s="2" t="n">
+      <c r="A166" s="1" t="n">
         <v>37621</v>
       </c>
       <c r="B166" t="n">
@@ -3803,7 +3764,7 @@
       </c>
     </row>
     <row r="167">
-      <c r="A167" s="2" t="n">
+      <c r="A167" s="1" t="n">
         <v>37652</v>
       </c>
       <c r="B167" t="n">
@@ -3832,7 +3793,7 @@
       </c>
     </row>
     <row r="168">
-      <c r="A168" s="2" t="n">
+      <c r="A168" s="1" t="n">
         <v>37680</v>
       </c>
       <c r="B168" t="n">
@@ -3861,7 +3822,7 @@
       </c>
     </row>
     <row r="169">
-      <c r="A169" s="2" t="n">
+      <c r="A169" s="1" t="n">
         <v>37711</v>
       </c>
       <c r="B169" t="n">
@@ -3890,7 +3851,7 @@
       </c>
     </row>
     <row r="170">
-      <c r="A170" s="2" t="n">
+      <c r="A170" s="1" t="n">
         <v>37741</v>
       </c>
       <c r="B170" t="n">
@@ -3919,7 +3880,7 @@
       </c>
     </row>
     <row r="171">
-      <c r="A171" s="2" t="n">
+      <c r="A171" s="1" t="n">
         <v>37772</v>
       </c>
       <c r="B171" t="n">
@@ -3948,7 +3909,7 @@
       </c>
     </row>
     <row r="172">
-      <c r="A172" s="2" t="n">
+      <c r="A172" s="1" t="n">
         <v>37802</v>
       </c>
       <c r="B172" t="n">
@@ -3977,7 +3938,7 @@
       </c>
     </row>
     <row r="173">
-      <c r="A173" s="2" t="n">
+      <c r="A173" s="1" t="n">
         <v>37833</v>
       </c>
       <c r="B173" t="n">
@@ -4006,7 +3967,7 @@
       </c>
     </row>
     <row r="174">
-      <c r="A174" s="2" t="n">
+      <c r="A174" s="1" t="n">
         <v>37864</v>
       </c>
       <c r="B174" t="n">
@@ -4035,7 +3996,7 @@
       </c>
     </row>
     <row r="175">
-      <c r="A175" s="2" t="n">
+      <c r="A175" s="1" t="n">
         <v>37894</v>
       </c>
       <c r="B175" t="n">
@@ -4064,7 +4025,7 @@
       </c>
     </row>
     <row r="176">
-      <c r="A176" s="2" t="n">
+      <c r="A176" s="1" t="n">
         <v>37925</v>
       </c>
       <c r="B176" t="n">
@@ -4093,7 +4054,7 @@
       </c>
     </row>
     <row r="177">
-      <c r="A177" s="2" t="n">
+      <c r="A177" s="1" t="n">
         <v>37955</v>
       </c>
       <c r="B177" t="n">
@@ -4122,7 +4083,7 @@
       </c>
     </row>
     <row r="178">
-      <c r="A178" s="2" t="n">
+      <c r="A178" s="1" t="n">
         <v>37986</v>
       </c>
       <c r="B178" t="n">
@@ -4151,7 +4112,7 @@
       </c>
     </row>
     <row r="179">
-      <c r="A179" s="2" t="n">
+      <c r="A179" s="1" t="n">
         <v>38017</v>
       </c>
       <c r="B179" t="n">
@@ -4180,7 +4141,7 @@
       </c>
     </row>
     <row r="180">
-      <c r="A180" s="2" t="n">
+      <c r="A180" s="1" t="n">
         <v>38046</v>
       </c>
       <c r="B180" t="n">
@@ -4209,7 +4170,7 @@
       </c>
     </row>
     <row r="181">
-      <c r="A181" s="2" t="n">
+      <c r="A181" s="1" t="n">
         <v>38077</v>
       </c>
       <c r="B181" t="n">
@@ -4238,7 +4199,7 @@
       </c>
     </row>
     <row r="182">
-      <c r="A182" s="2" t="n">
+      <c r="A182" s="1" t="n">
         <v>38107</v>
       </c>
       <c r="B182" t="n">
@@ -4267,7 +4228,7 @@
       </c>
     </row>
     <row r="183">
-      <c r="A183" s="2" t="n">
+      <c r="A183" s="1" t="n">
         <v>38138</v>
       </c>
       <c r="B183" t="n">
@@ -4296,7 +4257,7 @@
       </c>
     </row>
     <row r="184">
-      <c r="A184" s="2" t="n">
+      <c r="A184" s="1" t="n">
         <v>38168</v>
       </c>
       <c r="B184" t="n">
@@ -4325,7 +4286,7 @@
       </c>
     </row>
     <row r="185">
-      <c r="A185" s="2" t="n">
+      <c r="A185" s="1" t="n">
         <v>38199</v>
       </c>
       <c r="B185" t="n">
@@ -4354,7 +4315,7 @@
       </c>
     </row>
     <row r="186">
-      <c r="A186" s="2" t="n">
+      <c r="A186" s="1" t="n">
         <v>38230</v>
       </c>
       <c r="B186" t="n">
@@ -4383,7 +4344,7 @@
       </c>
     </row>
     <row r="187">
-      <c r="A187" s="2" t="n">
+      <c r="A187" s="1" t="n">
         <v>38260</v>
       </c>
       <c r="B187" t="n">
@@ -4412,7 +4373,7 @@
       </c>
     </row>
     <row r="188">
-      <c r="A188" s="2" t="n">
+      <c r="A188" s="1" t="n">
         <v>38291</v>
       </c>
       <c r="B188" t="n">
@@ -4441,7 +4402,7 @@
       </c>
     </row>
     <row r="189">
-      <c r="A189" s="2" t="n">
+      <c r="A189" s="1" t="n">
         <v>38321</v>
       </c>
       <c r="B189" t="n">
@@ -4470,7 +4431,7 @@
       </c>
     </row>
     <row r="190">
-      <c r="A190" s="2" t="n">
+      <c r="A190" s="1" t="n">
         <v>38352</v>
       </c>
       <c r="B190" t="n">
@@ -4499,7 +4460,7 @@
       </c>
     </row>
     <row r="191">
-      <c r="A191" s="2" t="n">
+      <c r="A191" s="1" t="n">
         <v>38383</v>
       </c>
       <c r="B191" t="n">
@@ -4528,7 +4489,7 @@
       </c>
     </row>
     <row r="192">
-      <c r="A192" s="2" t="n">
+      <c r="A192" s="1" t="n">
         <v>38411</v>
       </c>
       <c r="B192" t="n">
@@ -4557,7 +4518,7 @@
       </c>
     </row>
     <row r="193">
-      <c r="A193" s="2" t="n">
+      <c r="A193" s="1" t="n">
         <v>38442</v>
       </c>
       <c r="B193" t="n">
@@ -4586,7 +4547,7 @@
       </c>
     </row>
     <row r="194">
-      <c r="A194" s="2" t="n">
+      <c r="A194" s="1" t="n">
         <v>38472</v>
       </c>
       <c r="B194" t="n">
@@ -4615,7 +4576,7 @@
       </c>
     </row>
     <row r="195">
-      <c r="A195" s="2" t="n">
+      <c r="A195" s="1" t="n">
         <v>38503</v>
       </c>
       <c r="B195" t="n">
@@ -4644,7 +4605,7 @@
       </c>
     </row>
     <row r="196">
-      <c r="A196" s="2" t="n">
+      <c r="A196" s="1" t="n">
         <v>38533</v>
       </c>
       <c r="B196" t="n">
@@ -4673,7 +4634,7 @@
       </c>
     </row>
     <row r="197">
-      <c r="A197" s="2" t="n">
+      <c r="A197" s="1" t="n">
         <v>38564</v>
       </c>
       <c r="B197" t="n">
@@ -4702,7 +4663,7 @@
       </c>
     </row>
     <row r="198">
-      <c r="A198" s="2" t="n">
+      <c r="A198" s="1" t="n">
         <v>38595</v>
       </c>
       <c r="B198" t="n">
@@ -4731,7 +4692,7 @@
       </c>
     </row>
     <row r="199">
-      <c r="A199" s="2" t="n">
+      <c r="A199" s="1" t="n">
         <v>38625</v>
       </c>
       <c r="B199" t="n">
@@ -4760,7 +4721,7 @@
       </c>
     </row>
     <row r="200">
-      <c r="A200" s="2" t="n">
+      <c r="A200" s="1" t="n">
         <v>38656</v>
       </c>
       <c r="B200" t="n">
@@ -4789,7 +4750,7 @@
       </c>
     </row>
     <row r="201">
-      <c r="A201" s="2" t="n">
+      <c r="A201" s="1" t="n">
         <v>38686</v>
       </c>
       <c r="B201" t="n">
@@ -4818,7 +4779,7 @@
       </c>
     </row>
     <row r="202">
-      <c r="A202" s="2" t="n">
+      <c r="A202" s="1" t="n">
         <v>38717</v>
       </c>
       <c r="B202" t="n">
@@ -4847,7 +4808,7 @@
       </c>
     </row>
     <row r="203">
-      <c r="A203" s="2" t="n">
+      <c r="A203" s="1" t="n">
         <v>38748</v>
       </c>
       <c r="B203" t="n">
@@ -4876,7 +4837,7 @@
       </c>
     </row>
     <row r="204">
-      <c r="A204" s="2" t="n">
+      <c r="A204" s="1" t="n">
         <v>38776</v>
       </c>
       <c r="B204" t="n">
@@ -4905,7 +4866,7 @@
       </c>
     </row>
     <row r="205">
-      <c r="A205" s="2" t="n">
+      <c r="A205" s="1" t="n">
         <v>38807</v>
       </c>
       <c r="B205" t="n">
@@ -4934,7 +4895,7 @@
       </c>
     </row>
     <row r="206">
-      <c r="A206" s="2" t="n">
+      <c r="A206" s="1" t="n">
         <v>38837</v>
       </c>
       <c r="B206" t="n">
@@ -4963,7 +4924,7 @@
       </c>
     </row>
     <row r="207">
-      <c r="A207" s="2" t="n">
+      <c r="A207" s="1" t="n">
         <v>38868</v>
       </c>
       <c r="B207" t="n">
@@ -4992,7 +4953,7 @@
       </c>
     </row>
     <row r="208">
-      <c r="A208" s="2" t="n">
+      <c r="A208" s="1" t="n">
         <v>38898</v>
       </c>
       <c r="B208" t="n">
@@ -5021,7 +4982,7 @@
       </c>
     </row>
     <row r="209">
-      <c r="A209" s="2" t="n">
+      <c r="A209" s="1" t="n">
         <v>38929</v>
       </c>
       <c r="B209" t="n">
@@ -5050,7 +5011,7 @@
       </c>
     </row>
     <row r="210">
-      <c r="A210" s="2" t="n">
+      <c r="A210" s="1" t="n">
         <v>38960</v>
       </c>
       <c r="B210" t="n">
@@ -5079,7 +5040,7 @@
       </c>
     </row>
     <row r="211">
-      <c r="A211" s="2" t="n">
+      <c r="A211" s="1" t="n">
         <v>38990</v>
       </c>
       <c r="B211" t="n">
@@ -5108,7 +5069,7 @@
       </c>
     </row>
     <row r="212">
-      <c r="A212" s="2" t="n">
+      <c r="A212" s="1" t="n">
         <v>39021</v>
       </c>
       <c r="B212" t="n">
@@ -5137,7 +5098,7 @@
       </c>
     </row>
     <row r="213">
-      <c r="A213" s="2" t="n">
+      <c r="A213" s="1" t="n">
         <v>39051</v>
       </c>
       <c r="B213" t="n">
@@ -5166,7 +5127,7 @@
       </c>
     </row>
     <row r="214">
-      <c r="A214" s="2" t="n">
+      <c r="A214" s="1" t="n">
         <v>39082</v>
       </c>
       <c r="B214" t="n">
@@ -5195,7 +5156,7 @@
       </c>
     </row>
     <row r="215">
-      <c r="A215" s="2" t="n">
+      <c r="A215" s="1" t="n">
         <v>39113</v>
       </c>
       <c r="B215" t="n">
@@ -5224,7 +5185,7 @@
       </c>
     </row>
     <row r="216">
-      <c r="A216" s="2" t="n">
+      <c r="A216" s="1" t="n">
         <v>39141</v>
       </c>
       <c r="B216" t="n">
@@ -5253,7 +5214,7 @@
       </c>
     </row>
     <row r="217">
-      <c r="A217" s="2" t="n">
+      <c r="A217" s="1" t="n">
         <v>39172</v>
       </c>
       <c r="B217" t="n">
@@ -5282,7 +5243,7 @@
       </c>
     </row>
     <row r="218">
-      <c r="A218" s="2" t="n">
+      <c r="A218" s="1" t="n">
         <v>39202</v>
       </c>
       <c r="B218" t="n">
@@ -5311,7 +5272,7 @@
       </c>
     </row>
     <row r="219">
-      <c r="A219" s="2" t="n">
+      <c r="A219" s="1" t="n">
         <v>39233</v>
       </c>
       <c r="B219" t="n">
@@ -5340,7 +5301,7 @@
       </c>
     </row>
     <row r="220">
-      <c r="A220" s="2" t="n">
+      <c r="A220" s="1" t="n">
         <v>39263</v>
       </c>
       <c r="B220" t="n">
@@ -5369,7 +5330,7 @@
       </c>
     </row>
     <row r="221">
-      <c r="A221" s="2" t="n">
+      <c r="A221" s="1" t="n">
         <v>39294</v>
       </c>
       <c r="B221" t="n">
@@ -5398,7 +5359,7 @@
       </c>
     </row>
     <row r="222">
-      <c r="A222" s="2" t="n">
+      <c r="A222" s="1" t="n">
         <v>39325</v>
       </c>
       <c r="B222" t="n">
@@ -5427,7 +5388,7 @@
       </c>
     </row>
     <row r="223">
-      <c r="A223" s="2" t="n">
+      <c r="A223" s="1" t="n">
         <v>39355</v>
       </c>
       <c r="B223" t="n">
@@ -5456,7 +5417,7 @@
       </c>
     </row>
     <row r="224">
-      <c r="A224" s="2" t="n">
+      <c r="A224" s="1" t="n">
         <v>39386</v>
       </c>
       <c r="B224" t="n">
@@ -5485,7 +5446,7 @@
       </c>
     </row>
     <row r="225">
-      <c r="A225" s="2" t="n">
+      <c r="A225" s="1" t="n">
         <v>39416</v>
       </c>
       <c r="B225" t="n">
@@ -5514,7 +5475,7 @@
       </c>
     </row>
     <row r="226">
-      <c r="A226" s="2" t="n">
+      <c r="A226" s="1" t="n">
         <v>39447</v>
       </c>
       <c r="B226" t="n">
@@ -5543,7 +5504,7 @@
       </c>
     </row>
     <row r="227">
-      <c r="A227" s="2" t="n">
+      <c r="A227" s="1" t="n">
         <v>39478</v>
       </c>
       <c r="B227" t="n">
@@ -5572,7 +5533,7 @@
       </c>
     </row>
     <row r="228">
-      <c r="A228" s="2" t="n">
+      <c r="A228" s="1" t="n">
         <v>39507</v>
       </c>
       <c r="B228" t="n">
@@ -5601,7 +5562,7 @@
       </c>
     </row>
     <row r="229">
-      <c r="A229" s="2" t="n">
+      <c r="A229" s="1" t="n">
         <v>39538</v>
       </c>
       <c r="B229" t="n">
@@ -5630,7 +5591,7 @@
       </c>
     </row>
     <row r="230">
-      <c r="A230" s="2" t="n">
+      <c r="A230" s="1" t="n">
         <v>39568</v>
       </c>
       <c r="B230" t="n">
@@ -5659,7 +5620,7 @@
       </c>
     </row>
     <row r="231">
-      <c r="A231" s="2" t="n">
+      <c r="A231" s="1" t="n">
         <v>39599</v>
       </c>
       <c r="B231" t="n">
@@ -5688,7 +5649,7 @@
       </c>
     </row>
     <row r="232">
-      <c r="A232" s="2" t="n">
+      <c r="A232" s="1" t="n">
         <v>39629</v>
       </c>
       <c r="B232" t="n">
@@ -5717,7 +5678,7 @@
       </c>
     </row>
     <row r="233">
-      <c r="A233" s="2" t="n">
+      <c r="A233" s="1" t="n">
         <v>39660</v>
       </c>
       <c r="B233" t="n">
@@ -5746,7 +5707,7 @@
       </c>
     </row>
     <row r="234">
-      <c r="A234" s="2" t="n">
+      <c r="A234" s="1" t="n">
         <v>39691</v>
       </c>
       <c r="B234" t="n">
@@ -5775,7 +5736,7 @@
       </c>
     </row>
     <row r="235">
-      <c r="A235" s="2" t="n">
+      <c r="A235" s="1" t="n">
         <v>39721</v>
       </c>
       <c r="B235" t="n">
@@ -5802,7 +5763,7 @@
       </c>
     </row>
     <row r="236">
-      <c r="A236" s="2" t="n">
+      <c r="A236" s="1" t="n">
         <v>39752</v>
       </c>
       <c r="B236" t="n">
@@ -5831,7 +5792,7 @@
       </c>
     </row>
     <row r="237">
-      <c r="A237" s="2" t="n">
+      <c r="A237" s="1" t="n">
         <v>39782</v>
       </c>
       <c r="B237" t="n">
@@ -5860,7 +5821,7 @@
       </c>
     </row>
     <row r="238">
-      <c r="A238" s="2" t="n">
+      <c r="A238" s="1" t="n">
         <v>39813</v>
       </c>
       <c r="B238" t="n">
@@ -5889,7 +5850,7 @@
       </c>
     </row>
     <row r="239">
-      <c r="A239" s="2" t="n">
+      <c r="A239" s="1" t="n">
         <v>39844</v>
       </c>
       <c r="B239" t="n">
@@ -5918,7 +5879,7 @@
       </c>
     </row>
     <row r="240">
-      <c r="A240" s="2" t="n">
+      <c r="A240" s="1" t="n">
         <v>39872</v>
       </c>
       <c r="B240" t="n">
@@ -5947,7 +5908,7 @@
       </c>
     </row>
     <row r="241">
-      <c r="A241" s="2" t="n">
+      <c r="A241" s="1" t="n">
         <v>39903</v>
       </c>
       <c r="B241" t="n">
@@ -5976,7 +5937,7 @@
       </c>
     </row>
     <row r="242">
-      <c r="A242" s="2" t="n">
+      <c r="A242" s="1" t="n">
         <v>39933</v>
       </c>
       <c r="B242" t="inlineStr"/>
@@ -5989,7 +5950,7 @@
       <c r="I242" t="inlineStr"/>
     </row>
     <row r="243">
-      <c r="A243" s="2" t="n">
+      <c r="A243" s="1" t="n">
         <v>39964</v>
       </c>
       <c r="B243" t="n">
@@ -6018,7 +5979,7 @@
       </c>
     </row>
     <row r="244">
-      <c r="A244" s="2" t="n">
+      <c r="A244" s="1" t="n">
         <v>39994</v>
       </c>
       <c r="B244" t="n">
@@ -6047,7 +6008,7 @@
       </c>
     </row>
     <row r="245">
-      <c r="A245" s="2" t="n">
+      <c r="A245" s="1" t="n">
         <v>40025</v>
       </c>
       <c r="B245" t="n">
@@ -6076,7 +6037,7 @@
       </c>
     </row>
     <row r="246">
-      <c r="A246" s="2" t="n">
+      <c r="A246" s="1" t="n">
         <v>40056</v>
       </c>
       <c r="B246" t="n">
@@ -6105,7 +6066,7 @@
       </c>
     </row>
     <row r="247">
-      <c r="A247" s="2" t="n">
+      <c r="A247" s="1" t="n">
         <v>40086</v>
       </c>
       <c r="B247" t="n">
@@ -6134,7 +6095,7 @@
       </c>
     </row>
     <row r="248">
-      <c r="A248" s="2" t="n">
+      <c r="A248" s="1" t="n">
         <v>40117</v>
       </c>
       <c r="B248" t="n">
@@ -6163,7 +6124,7 @@
       </c>
     </row>
     <row r="249">
-      <c r="A249" s="2" t="n">
+      <c r="A249" s="1" t="n">
         <v>40147</v>
       </c>
       <c r="B249" t="n">
@@ -6192,7 +6153,7 @@
       </c>
     </row>
     <row r="250">
-      <c r="A250" s="2" t="n">
+      <c r="A250" s="1" t="n">
         <v>40178</v>
       </c>
       <c r="B250" t="n">
@@ -6221,7 +6182,7 @@
       </c>
     </row>
     <row r="251">
-      <c r="A251" s="2" t="n">
+      <c r="A251" s="1" t="n">
         <v>40209</v>
       </c>
       <c r="B251" t="n">
@@ -6250,7 +6211,7 @@
       </c>
     </row>
     <row r="252">
-      <c r="A252" s="2" t="n">
+      <c r="A252" s="1" t="n">
         <v>40237</v>
       </c>
       <c r="B252" t="n">
@@ -6279,7 +6240,7 @@
       </c>
     </row>
     <row r="253">
-      <c r="A253" s="2" t="n">
+      <c r="A253" s="1" t="n">
         <v>40268</v>
       </c>
       <c r="B253" t="n">
@@ -6308,7 +6269,7 @@
       </c>
     </row>
     <row r="254">
-      <c r="A254" s="2" t="n">
+      <c r="A254" s="1" t="n">
         <v>40298</v>
       </c>
       <c r="B254" t="n">
@@ -6337,7 +6298,7 @@
       </c>
     </row>
     <row r="255">
-      <c r="A255" s="2" t="n">
+      <c r="A255" s="1" t="n">
         <v>40329</v>
       </c>
       <c r="B255" t="n">
@@ -6366,7 +6327,7 @@
       </c>
     </row>
     <row r="256">
-      <c r="A256" s="2" t="n">
+      <c r="A256" s="1" t="n">
         <v>40359</v>
       </c>
       <c r="B256" t="n">
@@ -6395,7 +6356,7 @@
       </c>
     </row>
     <row r="257">
-      <c r="A257" s="2" t="n">
+      <c r="A257" s="1" t="n">
         <v>40390</v>
       </c>
       <c r="B257" t="n">
@@ -6424,7 +6385,7 @@
       </c>
     </row>
     <row r="258">
-      <c r="A258" s="2" t="n">
+      <c r="A258" s="1" t="n">
         <v>40421</v>
       </c>
       <c r="B258" t="n">
@@ -6453,7 +6414,7 @@
       </c>
     </row>
     <row r="259">
-      <c r="A259" s="2" t="n">
+      <c r="A259" s="1" t="n">
         <v>40451</v>
       </c>
       <c r="B259" t="n">
@@ -6482,7 +6443,7 @@
       </c>
     </row>
     <row r="260">
-      <c r="A260" s="2" t="n">
+      <c r="A260" s="1" t="n">
         <v>40482</v>
       </c>
       <c r="B260" t="n">
@@ -6511,7 +6472,7 @@
       </c>
     </row>
     <row r="261">
-      <c r="A261" s="2" t="n">
+      <c r="A261" s="1" t="n">
         <v>40512</v>
       </c>
       <c r="B261" t="n">
@@ -6540,7 +6501,7 @@
       </c>
     </row>
     <row r="262">
-      <c r="A262" s="2" t="n">
+      <c r="A262" s="1" t="n">
         <v>40543</v>
       </c>
       <c r="B262" t="n">
@@ -6569,7 +6530,7 @@
       </c>
     </row>
     <row r="263">
-      <c r="A263" s="2" t="n">
+      <c r="A263" s="1" t="n">
         <v>40574</v>
       </c>
       <c r="B263" t="inlineStr"/>
@@ -6582,7 +6543,7 @@
       <c r="I263" t="inlineStr"/>
     </row>
     <row r="264">
-      <c r="A264" s="2" t="n">
+      <c r="A264" s="1" t="n">
         <v>40602</v>
       </c>
       <c r="B264" t="n">
@@ -6611,7 +6572,7 @@
       </c>
     </row>
     <row r="265">
-      <c r="A265" s="2" t="n">
+      <c r="A265" s="1" t="n">
         <v>40633</v>
       </c>
       <c r="B265" t="n">
@@ -6640,7 +6601,7 @@
       </c>
     </row>
     <row r="266">
-      <c r="A266" s="2" t="n">
+      <c r="A266" s="1" t="n">
         <v>40663</v>
       </c>
       <c r="B266" t="n">
@@ -6669,7 +6630,7 @@
       </c>
     </row>
     <row r="267">
-      <c r="A267" s="2" t="n">
+      <c r="A267" s="1" t="n">
         <v>40694</v>
       </c>
       <c r="B267" t="n">
@@ -6698,7 +6659,7 @@
       </c>
     </row>
     <row r="268">
-      <c r="A268" s="2" t="n">
+      <c r="A268" s="1" t="n">
         <v>40724</v>
       </c>
       <c r="B268" t="n">
@@ -6727,7 +6688,7 @@
       </c>
     </row>
     <row r="269">
-      <c r="A269" s="2" t="n">
+      <c r="A269" s="1" t="n">
         <v>40755</v>
       </c>
       <c r="B269" t="n">
@@ -6756,7 +6717,7 @@
       </c>
     </row>
     <row r="270">
-      <c r="A270" s="2" t="n">
+      <c r="A270" s="1" t="n">
         <v>40786</v>
       </c>
       <c r="B270" t="n">
@@ -6785,7 +6746,7 @@
       </c>
     </row>
     <row r="271">
-      <c r="A271" s="2" t="n">
+      <c r="A271" s="1" t="n">
         <v>40816</v>
       </c>
       <c r="B271" t="n">
@@ -6814,7 +6775,7 @@
       </c>
     </row>
     <row r="272">
-      <c r="A272" s="2" t="n">
+      <c r="A272" s="1" t="n">
         <v>40847</v>
       </c>
       <c r="B272" t="n">
@@ -6843,7 +6804,7 @@
       </c>
     </row>
     <row r="273">
-      <c r="A273" s="2" t="n">
+      <c r="A273" s="1" t="n">
         <v>40877</v>
       </c>
       <c r="B273" t="n">
@@ -6872,7 +6833,7 @@
       </c>
     </row>
     <row r="274">
-      <c r="A274" s="2" t="n">
+      <c r="A274" s="1" t="n">
         <v>40908</v>
       </c>
       <c r="B274" t="n">
@@ -6901,7 +6862,7 @@
       </c>
     </row>
     <row r="275">
-      <c r="A275" s="2" t="n">
+      <c r="A275" s="1" t="n">
         <v>40939</v>
       </c>
       <c r="B275" t="n">
@@ -6930,7 +6891,7 @@
       </c>
     </row>
     <row r="276">
-      <c r="A276" s="2" t="n">
+      <c r="A276" s="1" t="n">
         <v>40968</v>
       </c>
       <c r="B276" t="n">
@@ -6959,7 +6920,7 @@
       </c>
     </row>
     <row r="277">
-      <c r="A277" s="2" t="n">
+      <c r="A277" s="1" t="n">
         <v>40999</v>
       </c>
       <c r="B277" t="n">
@@ -6988,7 +6949,7 @@
       </c>
     </row>
     <row r="278">
-      <c r="A278" s="2" t="n">
+      <c r="A278" s="1" t="n">
         <v>41029</v>
       </c>
       <c r="B278" t="n">
@@ -7017,7 +6978,7 @@
       </c>
     </row>
     <row r="279">
-      <c r="A279" s="2" t="n">
+      <c r="A279" s="1" t="n">
         <v>41060</v>
       </c>
       <c r="B279" t="n">
@@ -7046,7 +7007,7 @@
       </c>
     </row>
     <row r="280">
-      <c r="A280" s="2" t="n">
+      <c r="A280" s="1" t="n">
         <v>41090</v>
       </c>
       <c r="B280" t="n">
@@ -7075,7 +7036,7 @@
       </c>
     </row>
     <row r="281">
-      <c r="A281" s="2" t="n">
+      <c r="A281" s="1" t="n">
         <v>41121</v>
       </c>
       <c r="B281" t="n">
@@ -7104,7 +7065,7 @@
       </c>
     </row>
     <row r="282">
-      <c r="A282" s="2" t="n">
+      <c r="A282" s="1" t="n">
         <v>41152</v>
       </c>
       <c r="B282" t="n">
@@ -7133,7 +7094,7 @@
       </c>
     </row>
     <row r="283">
-      <c r="A283" s="2" t="n">
+      <c r="A283" s="1" t="n">
         <v>41182</v>
       </c>
       <c r="B283" t="n">
@@ -7162,7 +7123,7 @@
       </c>
     </row>
     <row r="284">
-      <c r="A284" s="2" t="n">
+      <c r="A284" s="1" t="n">
         <v>41213</v>
       </c>
       <c r="B284" t="n">
@@ -7191,7 +7152,7 @@
       </c>
     </row>
     <row r="285">
-      <c r="A285" s="2" t="n">
+      <c r="A285" s="1" t="n">
         <v>41243</v>
       </c>
       <c r="B285" t="n">
@@ -7220,7 +7181,7 @@
       </c>
     </row>
     <row r="286">
-      <c r="A286" s="2" t="n">
+      <c r="A286" s="1" t="n">
         <v>41274</v>
       </c>
       <c r="B286" t="n">
@@ -7249,7 +7210,7 @@
       </c>
     </row>
     <row r="287">
-      <c r="A287" s="2" t="n">
+      <c r="A287" s="1" t="n">
         <v>41305</v>
       </c>
       <c r="B287" t="n">
@@ -7278,7 +7239,7 @@
       </c>
     </row>
     <row r="288">
-      <c r="A288" s="2" t="n">
+      <c r="A288" s="1" t="n">
         <v>41333</v>
       </c>
       <c r="B288" t="n">
@@ -7307,7 +7268,7 @@
       </c>
     </row>
     <row r="289">
-      <c r="A289" s="2" t="n">
+      <c r="A289" s="1" t="n">
         <v>41364</v>
       </c>
       <c r="B289" t="n">
@@ -7336,7 +7297,7 @@
       </c>
     </row>
     <row r="290">
-      <c r="A290" s="2" t="n">
+      <c r="A290" s="1" t="n">
         <v>41394</v>
       </c>
       <c r="B290" t="n">
@@ -7365,7 +7326,7 @@
       </c>
     </row>
     <row r="291">
-      <c r="A291" s="2" t="n">
+      <c r="A291" s="1" t="n">
         <v>41425</v>
       </c>
       <c r="B291" t="n">
@@ -7394,7 +7355,7 @@
       </c>
     </row>
     <row r="292">
-      <c r="A292" s="2" t="n">
+      <c r="A292" s="1" t="n">
         <v>41455</v>
       </c>
       <c r="B292" t="n">
@@ -7423,7 +7384,7 @@
       </c>
     </row>
     <row r="293">
-      <c r="A293" s="2" t="n">
+      <c r="A293" s="1" t="n">
         <v>41486</v>
       </c>
       <c r="B293" t="n">
@@ -7452,7 +7413,7 @@
       </c>
     </row>
     <row r="294">
-      <c r="A294" s="2" t="n">
+      <c r="A294" s="1" t="n">
         <v>41517</v>
       </c>
       <c r="B294" t="n">
@@ -7481,7 +7442,7 @@
       </c>
     </row>
     <row r="295">
-      <c r="A295" s="2" t="n">
+      <c r="A295" s="1" t="n">
         <v>41547</v>
       </c>
       <c r="B295" t="n">
@@ -7510,7 +7471,7 @@
       </c>
     </row>
     <row r="296">
-      <c r="A296" s="2" t="n">
+      <c r="A296" s="1" t="n">
         <v>41578</v>
       </c>
       <c r="B296" t="n">
@@ -7539,7 +7500,7 @@
       </c>
     </row>
     <row r="297">
-      <c r="A297" s="2" t="n">
+      <c r="A297" s="1" t="n">
         <v>41608</v>
       </c>
       <c r="B297" t="n">
@@ -7568,7 +7529,7 @@
       </c>
     </row>
     <row r="298">
-      <c r="A298" s="2" t="n">
+      <c r="A298" s="1" t="n">
         <v>41639</v>
       </c>
       <c r="B298" t="n">
@@ -7597,7 +7558,7 @@
       </c>
     </row>
     <row r="299">
-      <c r="A299" s="2" t="n">
+      <c r="A299" s="1" t="n">
         <v>41670</v>
       </c>
       <c r="B299" t="n">
@@ -7626,7 +7587,7 @@
       </c>
     </row>
     <row r="300">
-      <c r="A300" s="2" t="n">
+      <c r="A300" s="1" t="n">
         <v>41698</v>
       </c>
       <c r="B300" t="n">
@@ -7655,7 +7616,7 @@
       </c>
     </row>
     <row r="301">
-      <c r="A301" s="2" t="n">
+      <c r="A301" s="1" t="n">
         <v>41729</v>
       </c>
       <c r="B301" t="n">
@@ -7684,7 +7645,7 @@
       </c>
     </row>
     <row r="302">
-      <c r="A302" s="2" t="n">
+      <c r="A302" s="1" t="n">
         <v>41759</v>
       </c>
       <c r="B302" t="n">
@@ -7713,7 +7674,7 @@
       </c>
     </row>
     <row r="303">
-      <c r="A303" s="2" t="n">
+      <c r="A303" s="1" t="n">
         <v>41790</v>
       </c>
       <c r="B303" t="n">
@@ -7742,7 +7703,7 @@
       </c>
     </row>
     <row r="304">
-      <c r="A304" s="2" t="n">
+      <c r="A304" s="1" t="n">
         <v>41820</v>
       </c>
       <c r="B304" t="n">
@@ -7771,7 +7732,7 @@
       </c>
     </row>
     <row r="305">
-      <c r="A305" s="2" t="n">
+      <c r="A305" s="1" t="n">
         <v>41851</v>
       </c>
       <c r="B305" t="n">
@@ -7800,7 +7761,7 @@
       </c>
     </row>
     <row r="306">
-      <c r="A306" s="2" t="n">
+      <c r="A306" s="1" t="n">
         <v>41882</v>
       </c>
       <c r="B306" t="n">
@@ -7829,7 +7790,7 @@
       </c>
     </row>
     <row r="307">
-      <c r="A307" s="2" t="n">
+      <c r="A307" s="1" t="n">
         <v>41912</v>
       </c>
       <c r="B307" t="n">
@@ -7858,7 +7819,7 @@
       </c>
     </row>
     <row r="308">
-      <c r="A308" s="2" t="n">
+      <c r="A308" s="1" t="n">
         <v>41943</v>
       </c>
       <c r="B308" t="n">
@@ -7887,7 +7848,7 @@
       </c>
     </row>
     <row r="309">
-      <c r="A309" s="2" t="n">
+      <c r="A309" s="1" t="n">
         <v>41973</v>
       </c>
       <c r="B309" t="n">
@@ -7916,7 +7877,7 @@
       </c>
     </row>
     <row r="310">
-      <c r="A310" s="2" t="n">
+      <c r="A310" s="1" t="n">
         <v>42004</v>
       </c>
       <c r="B310" t="n">
@@ -7945,7 +7906,7 @@
       </c>
     </row>
     <row r="311">
-      <c r="A311" s="2" t="n">
+      <c r="A311" s="1" t="n">
         <v>42035</v>
       </c>
       <c r="B311" t="n">
@@ -7974,7 +7935,7 @@
       </c>
     </row>
     <row r="312">
-      <c r="A312" s="2" t="n">
+      <c r="A312" s="1" t="n">
         <v>42063</v>
       </c>
       <c r="B312" t="n">
@@ -8003,7 +7964,7 @@
       </c>
     </row>
     <row r="313">
-      <c r="A313" s="2" t="n">
+      <c r="A313" s="1" t="n">
         <v>42094</v>
       </c>
       <c r="B313" t="n">
@@ -8032,7 +7993,7 @@
       </c>
     </row>
     <row r="314">
-      <c r="A314" s="2" t="n">
+      <c r="A314" s="1" t="n">
         <v>42124</v>
       </c>
       <c r="B314" t="n">
@@ -8061,7 +8022,7 @@
       </c>
     </row>
     <row r="315">
-      <c r="A315" s="2" t="n">
+      <c r="A315" s="1" t="n">
         <v>42155</v>
       </c>
       <c r="B315" t="n">
@@ -8090,7 +8051,7 @@
       </c>
     </row>
     <row r="316">
-      <c r="A316" s="2" t="n">
+      <c r="A316" s="1" t="n">
         <v>42185</v>
       </c>
       <c r="B316" t="n">
@@ -8119,7 +8080,7 @@
       </c>
     </row>
     <row r="317">
-      <c r="A317" s="2" t="n">
+      <c r="A317" s="1" t="n">
         <v>42216</v>
       </c>
       <c r="B317" t="n">
@@ -8148,7 +8109,7 @@
       </c>
     </row>
     <row r="318">
-      <c r="A318" s="2" t="n">
+      <c r="A318" s="1" t="n">
         <v>42247</v>
       </c>
       <c r="B318" t="n">
@@ -8177,7 +8138,7 @@
       </c>
     </row>
     <row r="319">
-      <c r="A319" s="2" t="n">
+      <c r="A319" s="1" t="n">
         <v>42277</v>
       </c>
       <c r="B319" t="n">
@@ -8206,7 +8167,7 @@
       </c>
     </row>
     <row r="320">
-      <c r="A320" s="2" t="n">
+      <c r="A320" s="1" t="n">
         <v>42308</v>
       </c>
       <c r="B320" t="n">
@@ -8235,7 +8196,7 @@
       </c>
     </row>
     <row r="321">
-      <c r="A321" s="2" t="n">
+      <c r="A321" s="1" t="n">
         <v>42338</v>
       </c>
       <c r="B321" t="n">
@@ -8264,7 +8225,7 @@
       </c>
     </row>
     <row r="322">
-      <c r="A322" s="2" t="n">
+      <c r="A322" s="1" t="n">
         <v>42369</v>
       </c>
       <c r="B322" t="n">
@@ -8293,7 +8254,7 @@
       </c>
     </row>
     <row r="323">
-      <c r="A323" s="2" t="n">
+      <c r="A323" s="1" t="n">
         <v>42400</v>
       </c>
       <c r="B323" t="n">
@@ -8322,7 +8283,7 @@
       </c>
     </row>
     <row r="324">
-      <c r="A324" s="2" t="n">
+      <c r="A324" s="1" t="n">
         <v>42429</v>
       </c>
       <c r="B324" t="n">
@@ -8351,7 +8312,7 @@
       </c>
     </row>
     <row r="325">
-      <c r="A325" s="2" t="n">
+      <c r="A325" s="1" t="n">
         <v>42460</v>
       </c>
       <c r="B325" t="n">
@@ -8380,7 +8341,7 @@
       </c>
     </row>
     <row r="326">
-      <c r="A326" s="2" t="n">
+      <c r="A326" s="1" t="n">
         <v>42490</v>
       </c>
       <c r="B326" t="n">
@@ -8409,7 +8370,7 @@
       </c>
     </row>
     <row r="327">
-      <c r="A327" s="2" t="n">
+      <c r="A327" s="1" t="n">
         <v>42521</v>
       </c>
       <c r="B327" t="n">
@@ -8438,7 +8399,7 @@
       </c>
     </row>
     <row r="328">
-      <c r="A328" s="2" t="n">
+      <c r="A328" s="1" t="n">
         <v>42551</v>
       </c>
       <c r="B328" t="n">
@@ -8467,7 +8428,7 @@
       </c>
     </row>
     <row r="329">
-      <c r="A329" s="2" t="n">
+      <c r="A329" s="1" t="n">
         <v>42582</v>
       </c>
       <c r="B329" t="n">
@@ -8496,7 +8457,7 @@
       </c>
     </row>
     <row r="330">
-      <c r="A330" s="2" t="n">
+      <c r="A330" s="1" t="n">
         <v>42613</v>
       </c>
       <c r="B330" t="n">
@@ -8525,7 +8486,7 @@
       </c>
     </row>
     <row r="331">
-      <c r="A331" s="2" t="n">
+      <c r="A331" s="1" t="n">
         <v>42643</v>
       </c>
       <c r="B331" t="n">
@@ -8554,7 +8515,7 @@
       </c>
     </row>
     <row r="332">
-      <c r="A332" s="2" t="n">
+      <c r="A332" s="1" t="n">
         <v>42674</v>
       </c>
       <c r="B332" t="n">
@@ -8583,7 +8544,7 @@
       </c>
     </row>
     <row r="333">
-      <c r="A333" s="2" t="n">
+      <c r="A333" s="1" t="n">
         <v>42704</v>
       </c>
       <c r="B333" t="n">
@@ -8612,7 +8573,7 @@
       </c>
     </row>
     <row r="334">
-      <c r="A334" s="2" t="n">
+      <c r="A334" s="1" t="n">
         <v>42735</v>
       </c>
       <c r="B334" t="n">
@@ -8641,7 +8602,7 @@
       </c>
     </row>
     <row r="335">
-      <c r="A335" s="2" t="n">
+      <c r="A335" s="1" t="n">
         <v>42766</v>
       </c>
       <c r="B335" t="n">
@@ -8670,7 +8631,7 @@
       </c>
     </row>
     <row r="336">
-      <c r="A336" s="2" t="n">
+      <c r="A336" s="1" t="n">
         <v>42794</v>
       </c>
       <c r="B336" t="n">
@@ -8699,7 +8660,7 @@
       </c>
     </row>
     <row r="337">
-      <c r="A337" s="2" t="n">
+      <c r="A337" s="1" t="n">
         <v>42825</v>
       </c>
       <c r="B337" t="n">
@@ -8728,7 +8689,7 @@
       </c>
     </row>
     <row r="338">
-      <c r="A338" s="2" t="n">
+      <c r="A338" s="1" t="n">
         <v>42855</v>
       </c>
       <c r="B338" t="n">
@@ -8757,7 +8718,7 @@
       </c>
     </row>
     <row r="339">
-      <c r="A339" s="2" t="n">
+      <c r="A339" s="1" t="n">
         <v>42886</v>
       </c>
       <c r="B339" t="n">
@@ -8786,7 +8747,7 @@
       </c>
     </row>
     <row r="340">
-      <c r="A340" s="2" t="n">
+      <c r="A340" s="1" t="n">
         <v>42916</v>
       </c>
       <c r="B340" t="n">
@@ -8815,7 +8776,7 @@
       </c>
     </row>
     <row r="341">
-      <c r="A341" s="2" t="n">
+      <c r="A341" s="1" t="n">
         <v>42947</v>
       </c>
       <c r="B341" t="n">
@@ -8844,7 +8805,7 @@
       </c>
     </row>
     <row r="342">
-      <c r="A342" s="2" t="n">
+      <c r="A342" s="1" t="n">
         <v>42978</v>
       </c>
       <c r="B342" t="n">
@@ -8873,7 +8834,7 @@
       </c>
     </row>
     <row r="343">
-      <c r="A343" s="2" t="n">
+      <c r="A343" s="1" t="n">
         <v>43008</v>
       </c>
       <c r="B343" t="n">
@@ -8902,7 +8863,7 @@
       </c>
     </row>
     <row r="344">
-      <c r="A344" s="2" t="n">
+      <c r="A344" s="1" t="n">
         <v>43039</v>
       </c>
       <c r="B344" t="n">
@@ -8931,7 +8892,7 @@
       </c>
     </row>
     <row r="345">
-      <c r="A345" s="2" t="n">
+      <c r="A345" s="1" t="n">
         <v>43069</v>
       </c>
       <c r="B345" t="n">
@@ -8960,7 +8921,7 @@
       </c>
     </row>
     <row r="346">
-      <c r="A346" s="2" t="n">
+      <c r="A346" s="1" t="n">
         <v>43100</v>
       </c>
       <c r="B346" t="n">
@@ -8989,7 +8950,7 @@
       </c>
     </row>
     <row r="347">
-      <c r="A347" s="2" t="n">
+      <c r="A347" s="1" t="n">
         <v>43131</v>
       </c>
       <c r="B347" t="n">
@@ -9018,7 +8979,7 @@
       </c>
     </row>
     <row r="348">
-      <c r="A348" s="2" t="n">
+      <c r="A348" s="1" t="n">
         <v>43159</v>
       </c>
       <c r="B348" t="n">
@@ -9047,7 +9008,7 @@
       </c>
     </row>
     <row r="349">
-      <c r="A349" s="2" t="n">
+      <c r="A349" s="1" t="n">
         <v>43190</v>
       </c>
       <c r="B349" t="n">
@@ -9076,7 +9037,7 @@
       </c>
     </row>
     <row r="350">
-      <c r="A350" s="2" t="n">
+      <c r="A350" s="1" t="n">
         <v>43220</v>
       </c>
       <c r="B350" t="n">
@@ -9105,7 +9066,7 @@
       </c>
     </row>
     <row r="351">
-      <c r="A351" s="2" t="n">
+      <c r="A351" s="1" t="n">
         <v>43251</v>
       </c>
       <c r="B351" t="n">
@@ -9134,7 +9095,7 @@
       </c>
     </row>
     <row r="352">
-      <c r="A352" s="2" t="n">
+      <c r="A352" s="1" t="n">
         <v>43281</v>
       </c>
       <c r="B352" t="n">
@@ -9163,7 +9124,7 @@
       </c>
     </row>
     <row r="353">
-      <c r="A353" s="2" t="n">
+      <c r="A353" s="1" t="n">
         <v>43312</v>
       </c>
       <c r="B353" t="n">
@@ -9192,7 +9153,7 @@
       </c>
     </row>
     <row r="354">
-      <c r="A354" s="2" t="n">
+      <c r="A354" s="1" t="n">
         <v>43343</v>
       </c>
       <c r="B354" t="n">
@@ -9221,7 +9182,7 @@
       </c>
     </row>
     <row r="355">
-      <c r="A355" s="2" t="n">
+      <c r="A355" s="1" t="n">
         <v>43373</v>
       </c>
       <c r="B355" t="n">
@@ -9250,7 +9211,7 @@
       </c>
     </row>
     <row r="356">
-      <c r="A356" s="2" t="n">
+      <c r="A356" s="1" t="n">
         <v>43404</v>
       </c>
       <c r="B356" t="n">
@@ -9279,7 +9240,7 @@
       </c>
     </row>
     <row r="357">
-      <c r="A357" s="2" t="n">
+      <c r="A357" s="1" t="n">
         <v>43434</v>
       </c>
       <c r="B357" t="n">
@@ -9308,7 +9269,7 @@
       </c>
     </row>
     <row r="358">
-      <c r="A358" s="2" t="n">
+      <c r="A358" s="1" t="n">
         <v>43465</v>
       </c>
       <c r="B358" t="n">
@@ -9337,7 +9298,7 @@
       </c>
     </row>
     <row r="359">
-      <c r="A359" s="2" t="n">
+      <c r="A359" s="1" t="n">
         <v>43496</v>
       </c>
       <c r="B359" t="n">
@@ -9366,7 +9327,7 @@
       </c>
     </row>
     <row r="360">
-      <c r="A360" s="2" t="n">
+      <c r="A360" s="1" t="n">
         <v>43524</v>
       </c>
       <c r="B360" t="n">
@@ -9395,7 +9356,7 @@
       </c>
     </row>
     <row r="361">
-      <c r="A361" s="2" t="n">
+      <c r="A361" s="1" t="n">
         <v>43555</v>
       </c>
       <c r="B361" t="n">
@@ -9424,7 +9385,7 @@
       </c>
     </row>
     <row r="362">
-      <c r="A362" s="2" t="n">
+      <c r="A362" s="1" t="n">
         <v>43585</v>
       </c>
       <c r="B362" t="n">
@@ -9453,7 +9414,7 @@
       </c>
     </row>
     <row r="363">
-      <c r="A363" s="2" t="n">
+      <c r="A363" s="1" t="n">
         <v>43616</v>
       </c>
       <c r="B363" t="n">
@@ -9482,7 +9443,7 @@
       </c>
     </row>
     <row r="364">
-      <c r="A364" s="2" t="n">
+      <c r="A364" s="1" t="n">
         <v>43646</v>
       </c>
       <c r="B364" t="n">
@@ -9511,7 +9472,7 @@
       </c>
     </row>
     <row r="365">
-      <c r="A365" s="2" t="n">
+      <c r="A365" s="1" t="n">
         <v>43677</v>
       </c>
       <c r="B365" t="n">
@@ -9540,7 +9501,7 @@
       </c>
     </row>
     <row r="366">
-      <c r="A366" s="2" t="n">
+      <c r="A366" s="1" t="n">
         <v>43708</v>
       </c>
       <c r="B366" t="n">
@@ -9569,7 +9530,7 @@
       </c>
     </row>
     <row r="367">
-      <c r="A367" s="2" t="n">
+      <c r="A367" s="1" t="n">
         <v>43738</v>
       </c>
       <c r="B367" t="n">
@@ -9598,7 +9559,7 @@
       </c>
     </row>
     <row r="368">
-      <c r="A368" s="2" t="n">
+      <c r="A368" s="1" t="n">
         <v>43769</v>
       </c>
       <c r="B368" t="n">
@@ -9627,7 +9588,7 @@
       </c>
     </row>
     <row r="369">
-      <c r="A369" s="2" t="n">
+      <c r="A369" s="1" t="n">
         <v>43799</v>
       </c>
       <c r="B369" t="n">
@@ -9656,7 +9617,7 @@
       </c>
     </row>
     <row r="370">
-      <c r="A370" s="2" t="n">
+      <c r="A370" s="1" t="n">
         <v>43830</v>
       </c>
       <c r="B370" t="n">
@@ -9685,7 +9646,7 @@
       </c>
     </row>
     <row r="371">
-      <c r="A371" s="2" t="n">
+      <c r="A371" s="1" t="n">
         <v>43861</v>
       </c>
       <c r="B371" t="n">
@@ -9714,7 +9675,7 @@
       </c>
     </row>
     <row r="372">
-      <c r="A372" s="2" t="n">
+      <c r="A372" s="1" t="n">
         <v>43890</v>
       </c>
       <c r="B372" t="n">
@@ -9743,7 +9704,7 @@
       </c>
     </row>
     <row r="373">
-      <c r="A373" s="2" t="n">
+      <c r="A373" s="1" t="n">
         <v>43921</v>
       </c>
       <c r="B373" t="n">
@@ -9772,7 +9733,7 @@
       </c>
     </row>
     <row r="374">
-      <c r="A374" s="2" t="n">
+      <c r="A374" s="1" t="n">
         <v>43951</v>
       </c>
       <c r="B374" t="n">
@@ -9801,7 +9762,7 @@
       </c>
     </row>
     <row r="375">
-      <c r="A375" s="2" t="n">
+      <c r="A375" s="1" t="n">
         <v>43982</v>
       </c>
       <c r="B375" t="n">
@@ -9830,7 +9791,7 @@
       </c>
     </row>
     <row r="376">
-      <c r="A376" s="2" t="n">
+      <c r="A376" s="1" t="n">
         <v>44012</v>
       </c>
       <c r="B376" t="n">
@@ -9859,7 +9820,7 @@
       </c>
     </row>
     <row r="377">
-      <c r="A377" s="2" t="n">
+      <c r="A377" s="1" t="n">
         <v>44043</v>
       </c>
       <c r="B377" t="n">
@@ -9888,7 +9849,7 @@
       </c>
     </row>
     <row r="378">
-      <c r="A378" s="2" t="n">
+      <c r="A378" s="1" t="n">
         <v>44074</v>
       </c>
       <c r="B378" t="n">
@@ -9917,7 +9878,7 @@
       </c>
     </row>
     <row r="379">
-      <c r="A379" s="2" t="n">
+      <c r="A379" s="1" t="n">
         <v>44104</v>
       </c>
       <c r="B379" t="n">
@@ -9946,7 +9907,7 @@
       </c>
     </row>
     <row r="380">
-      <c r="A380" s="2" t="n">
+      <c r="A380" s="1" t="n">
         <v>44135</v>
       </c>
       <c r="B380" t="n">
@@ -9975,7 +9936,7 @@
       </c>
     </row>
     <row r="381">
-      <c r="A381" s="2" t="n">
+      <c r="A381" s="1" t="n">
         <v>44165</v>
       </c>
       <c r="B381" t="n">
@@ -10004,7 +9965,7 @@
       </c>
     </row>
     <row r="382">
-      <c r="A382" s="2" t="n">
+      <c r="A382" s="1" t="n">
         <v>44196</v>
       </c>
       <c r="B382" t="n">
@@ -10033,7 +9994,7 @@
       </c>
     </row>
     <row r="383">
-      <c r="A383" s="2" t="n">
+      <c r="A383" s="1" t="n">
         <v>44227</v>
       </c>
       <c r="B383" t="n">
@@ -10062,7 +10023,7 @@
       </c>
     </row>
     <row r="384">
-      <c r="A384" s="2" t="n">
+      <c r="A384" s="1" t="n">
         <v>44255</v>
       </c>
       <c r="B384" t="n">
@@ -10091,7 +10052,7 @@
       </c>
     </row>
     <row r="385">
-      <c r="A385" s="2" t="n">
+      <c r="A385" s="1" t="n">
         <v>44286</v>
       </c>
       <c r="B385" t="n">
@@ -10120,7 +10081,7 @@
       </c>
     </row>
     <row r="386">
-      <c r="A386" s="2" t="n">
+      <c r="A386" s="1" t="n">
         <v>44316</v>
       </c>
       <c r="B386" t="n">
@@ -10149,7 +10110,7 @@
       </c>
     </row>
     <row r="387">
-      <c r="A387" s="2" t="n">
+      <c r="A387" s="1" t="n">
         <v>44347</v>
       </c>
       <c r="B387" t="n">
@@ -10178,7 +10139,7 @@
       </c>
     </row>
     <row r="388">
-      <c r="A388" s="2" t="n">
+      <c r="A388" s="1" t="n">
         <v>44377</v>
       </c>
       <c r="B388" t="n">
@@ -10207,7 +10168,7 @@
       </c>
     </row>
     <row r="389">
-      <c r="A389" s="2" t="n">
+      <c r="A389" s="1" t="n">
         <v>44408</v>
       </c>
       <c r="B389" t="n">
@@ -10236,7 +10197,7 @@
       </c>
     </row>
     <row r="390">
-      <c r="A390" s="2" t="n">
+      <c r="A390" s="1" t="n">
         <v>44439</v>
       </c>
       <c r="B390" t="n">
@@ -10265,7 +10226,7 @@
       </c>
     </row>
     <row r="391">
-      <c r="A391" s="2" t="n">
+      <c r="A391" s="1" t="n">
         <v>44469</v>
       </c>
       <c r="B391" t="n">
@@ -10294,7 +10255,7 @@
       </c>
     </row>
     <row r="392">
-      <c r="A392" s="2" t="n">
+      <c r="A392" s="1" t="n">
         <v>44500</v>
       </c>
       <c r="B392" t="n">
@@ -10323,7 +10284,7 @@
       </c>
     </row>
     <row r="393">
-      <c r="A393" s="2" t="n">
+      <c r="A393" s="1" t="n">
         <v>44530</v>
       </c>
       <c r="B393" t="n">
@@ -10352,7 +10313,7 @@
       </c>
     </row>
     <row r="394">
-      <c r="A394" s="2" t="n">
+      <c r="A394" s="1" t="n">
         <v>44561</v>
       </c>
       <c r="B394" t="n">
@@ -10381,7 +10342,7 @@
       </c>
     </row>
     <row r="395">
-      <c r="A395" s="2" t="n">
+      <c r="A395" s="1" t="n">
         <v>44592</v>
       </c>
       <c r="B395" t="n">
@@ -10410,7 +10371,7 @@
       </c>
     </row>
     <row r="396">
-      <c r="A396" s="2" t="n">
+      <c r="A396" s="1" t="n">
         <v>44620</v>
       </c>
       <c r="B396" t="n">
@@ -10439,7 +10400,7 @@
       </c>
     </row>
     <row r="397">
-      <c r="A397" s="2" t="n">
+      <c r="A397" s="1" t="n">
         <v>44651</v>
       </c>
       <c r="B397" t="n">
@@ -10468,7 +10429,7 @@
       </c>
     </row>
     <row r="398">
-      <c r="A398" s="2" t="n">
+      <c r="A398" s="1" t="n">
         <v>44681</v>
       </c>
       <c r="B398" t="n">
@@ -10497,7 +10458,7 @@
       </c>
     </row>
     <row r="399">
-      <c r="A399" s="2" t="n">
+      <c r="A399" s="1" t="n">
         <v>44712</v>
       </c>
       <c r="B399" t="n">
@@ -10526,7 +10487,7 @@
       </c>
     </row>
     <row r="400">
-      <c r="A400" s="2" t="n">
+      <c r="A400" s="1" t="n">
         <v>44742</v>
       </c>
       <c r="B400" t="n">
@@ -10555,7 +10516,7 @@
       </c>
     </row>
     <row r="401">
-      <c r="A401" s="2" t="n">
+      <c r="A401" s="1" t="n">
         <v>44773</v>
       </c>
       <c r="B401" t="n">
@@ -10584,7 +10545,7 @@
       </c>
     </row>
     <row r="402">
-      <c r="A402" s="2" t="n">
+      <c r="A402" s="1" t="n">
         <v>44804</v>
       </c>
       <c r="B402" t="n">
@@ -10613,7 +10574,7 @@
       </c>
     </row>
     <row r="403">
-      <c r="A403" s="2" t="n">
+      <c r="A403" s="1" t="n">
         <v>44834</v>
       </c>
       <c r="B403" t="n">
@@ -10642,7 +10603,7 @@
       </c>
     </row>
     <row r="404">
-      <c r="A404" s="2" t="n">
+      <c r="A404" s="1" t="n">
         <v>44865</v>
       </c>
       <c r="B404" t="n">
@@ -10671,7 +10632,7 @@
       </c>
     </row>
     <row r="405">
-      <c r="A405" s="2" t="n">
+      <c r="A405" s="1" t="n">
         <v>44895</v>
       </c>
       <c r="B405" t="n">
@@ -10700,7 +10661,7 @@
       </c>
     </row>
     <row r="406">
-      <c r="A406" s="2" t="n">
+      <c r="A406" s="1" t="n">
         <v>44926</v>
       </c>
       <c r="B406" t="n">
@@ -10729,7 +10690,7 @@
       </c>
     </row>
     <row r="407">
-      <c r="A407" s="2" t="n">
+      <c r="A407" s="1" t="n">
         <v>44957</v>
       </c>
       <c r="B407" t="n">
@@ -10758,7 +10719,7 @@
       </c>
     </row>
     <row r="408">
-      <c r="A408" s="2" t="n">
+      <c r="A408" s="1" t="n">
         <v>44985</v>
       </c>
       <c r="B408" t="n">
@@ -10787,7 +10748,7 @@
       </c>
     </row>
     <row r="409">
-      <c r="A409" s="2" t="n">
+      <c r="A409" s="1" t="n">
         <v>45016</v>
       </c>
       <c r="B409" t="n">
@@ -10816,7 +10777,7 @@
       </c>
     </row>
     <row r="410">
-      <c r="A410" s="2" t="n">
+      <c r="A410" s="1" t="n">
         <v>45046</v>
       </c>
       <c r="B410" t="n">
@@ -10845,7 +10806,7 @@
       </c>
     </row>
     <row r="411">
-      <c r="A411" s="2" t="n">
+      <c r="A411" s="1" t="n">
         <v>45077</v>
       </c>
       <c r="B411" t="n">
@@ -10874,7 +10835,7 @@
       </c>
     </row>
     <row r="412">
-      <c r="A412" s="2" t="n">
+      <c r="A412" s="1" t="n">
         <v>45107</v>
       </c>
       <c r="B412" t="n">
@@ -10903,7 +10864,7 @@
       </c>
     </row>
     <row r="413">
-      <c r="A413" s="2" t="n">
+      <c r="A413" s="1" t="n">
         <v>45138</v>
       </c>
       <c r="B413" t="n">
@@ -10932,7 +10893,7 @@
       </c>
     </row>
     <row r="414">
-      <c r="A414" s="2" t="n">
+      <c r="A414" s="1" t="n">
         <v>45169</v>
       </c>
       <c r="B414" t="n">
@@ -10961,7 +10922,7 @@
       </c>
     </row>
     <row r="415">
-      <c r="A415" s="2" t="n">
+      <c r="A415" s="1" t="n">
         <v>45199</v>
       </c>
       <c r="B415" t="n">
@@ -10990,7 +10951,7 @@
       </c>
     </row>
     <row r="416">
-      <c r="A416" s="2" t="n">
+      <c r="A416" s="1" t="n">
         <v>45230</v>
       </c>
       <c r="B416" t="n">
@@ -11019,7 +10980,7 @@
       </c>
     </row>
     <row r="417">
-      <c r="A417" s="2" t="n">
+      <c r="A417" s="1" t="n">
         <v>45260</v>
       </c>
       <c r="B417" t="n">
@@ -11048,7 +11009,7 @@
       </c>
     </row>
     <row r="418">
-      <c r="A418" s="2" t="n">
+      <c r="A418" s="1" t="n">
         <v>45291</v>
       </c>
       <c r="B418" t="n">
@@ -11077,7 +11038,7 @@
       </c>
     </row>
     <row r="419">
-      <c r="A419" s="2" t="n">
+      <c r="A419" s="1" t="n">
         <v>45322</v>
       </c>
       <c r="B419" t="n">
@@ -11106,7 +11067,7 @@
       </c>
     </row>
     <row r="420">
-      <c r="A420" s="2" t="n">
+      <c r="A420" s="1" t="n">
         <v>45351</v>
       </c>
       <c r="B420" t="n">
@@ -11135,7 +11096,7 @@
       </c>
     </row>
     <row r="421">
-      <c r="A421" s="2" t="n">
+      <c r="A421" s="1" t="n">
         <v>45382</v>
       </c>
       <c r="B421" t="n">
@@ -11164,7 +11125,7 @@
       </c>
     </row>
     <row r="422">
-      <c r="A422" s="2" t="n">
+      <c r="A422" s="1" t="n">
         <v>45412</v>
       </c>
       <c r="B422" t="n">
@@ -11193,7 +11154,7 @@
       </c>
     </row>
     <row r="423">
-      <c r="A423" s="2" t="n">
+      <c r="A423" s="1" t="n">
         <v>45443</v>
       </c>
       <c r="B423" t="n">
@@ -11222,7 +11183,7 @@
       </c>
     </row>
     <row r="424">
-      <c r="A424" s="2" t="n">
+      <c r="A424" s="1" t="n">
         <v>45473</v>
       </c>
       <c r="B424" t="n">
@@ -11251,7 +11212,7 @@
       </c>
     </row>
     <row r="425">
-      <c r="A425" s="2" t="n">
+      <c r="A425" s="1" t="n">
         <v>45504</v>
       </c>
       <c r="B425" t="n">
@@ -11280,7 +11241,7 @@
       </c>
     </row>
     <row r="426">
-      <c r="A426" s="2" t="n">
+      <c r="A426" s="1" t="n">
         <v>45535</v>
       </c>
       <c r="B426" t="n">
@@ -11309,7 +11270,7 @@
       </c>
     </row>
     <row r="427">
-      <c r="A427" s="2" t="n">
+      <c r="A427" s="1" t="n">
         <v>45565</v>
       </c>
       <c r="B427" t="n">
@@ -11338,7 +11299,7 @@
       </c>
     </row>
     <row r="428">
-      <c r="A428" s="2" t="n">
+      <c r="A428" s="1" t="n">
         <v>45596</v>
       </c>
       <c r="B428" t="n">
@@ -11367,7 +11328,7 @@
       </c>
     </row>
     <row r="429">
-      <c r="A429" s="2" t="n">
+      <c r="A429" s="1" t="n">
         <v>45626</v>
       </c>
       <c r="B429" t="n">
@@ -11396,7 +11357,7 @@
       </c>
     </row>
     <row r="430">
-      <c r="A430" s="2" t="n">
+      <c r="A430" s="1" t="n">
         <v>45657</v>
       </c>
       <c r="B430" t="n">
@@ -11425,7 +11386,7 @@
       </c>
     </row>
     <row r="431">
-      <c r="A431" s="2" t="n">
+      <c r="A431" s="1" t="n">
         <v>45688</v>
       </c>
       <c r="B431" t="n">
@@ -11454,7 +11415,7 @@
       </c>
     </row>
     <row r="432">
-      <c r="A432" s="2" t="n">
+      <c r="A432" s="1" t="n">
         <v>45716</v>
       </c>
       <c r="B432" t="n">
@@ -11483,7 +11444,7 @@
       </c>
     </row>
     <row r="433">
-      <c r="A433" s="2" t="n">
+      <c r="A433" s="1" t="n">
         <v>45747</v>
       </c>
       <c r="B433" t="n">
@@ -11512,7 +11473,7 @@
       </c>
     </row>
     <row r="434">
-      <c r="A434" s="2" t="n">
+      <c r="A434" s="1" t="n">
         <v>45777</v>
       </c>
       <c r="B434" t="n">
@@ -11541,7 +11502,7 @@
       </c>
     </row>
     <row r="435">
-      <c r="A435" s="2" t="n">
+      <c r="A435" s="1" t="n">
         <v>45808</v>
       </c>
       <c r="B435" t="n">
@@ -11570,7 +11531,7 @@
       </c>
     </row>
     <row r="436">
-      <c r="A436" s="2" t="n">
+      <c r="A436" s="1" t="n">
         <v>45838</v>
       </c>
       <c r="B436" t="n">
@@ -11599,7 +11560,7 @@
       </c>
     </row>
     <row r="437">
-      <c r="A437" s="2" t="n">
+      <c r="A437" s="1" t="n">
         <v>45869</v>
       </c>
       <c r="B437" t="n">
@@ -11628,7 +11589,7 @@
       </c>
     </row>
     <row r="438">
-      <c r="A438" s="2" t="n">
+      <c r="A438" s="1" t="n">
         <v>45900</v>
       </c>
       <c r="B438" t="n">
@@ -11654,6 +11615,35 @@
       </c>
       <c r="I438" t="n">
         <v>45.45454545454545</v>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" s="1" t="n">
+        <v>45930</v>
+      </c>
+      <c r="B439" t="n">
+        <v>66.66666666666666</v>
+      </c>
+      <c r="C439" t="n">
+        <v>91.66666666666666</v>
+      </c>
+      <c r="D439" t="n">
+        <v>47.36842105263158</v>
+      </c>
+      <c r="E439" t="n">
+        <v>41.17647058823529</v>
+      </c>
+      <c r="F439" t="n">
+        <v>78.57142857142857</v>
+      </c>
+      <c r="G439" t="n">
+        <v>69.23076923076923</v>
+      </c>
+      <c r="H439" t="n">
+        <v>42.10526315789473</v>
+      </c>
+      <c r="I439" t="n">
+        <v>46.15384615384615</v>
       </c>
     </row>
   </sheetData>

</xml_diff>